<commit_message>
Adding variable names to spreadsheet
</commit_message>
<xml_diff>
--- a/data-phi-free/raw/renaming-rules/renaming-rules.xlsx
+++ b/data-phi-free/raw/renaming-rules/renaming-rules.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koval_000\Documents\GitHub\HRS\data-phi-free\raw\renaming-rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cassandrabrown/Github/HRS/data-phi-free/raw/renaming-rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13215"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="loneliness" sheetId="1" r:id="rId1"/>
+    <sheet name="lifesatisfaction" sheetId="2" r:id="rId2"/>
+    <sheet name="socialnetwork" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">loneliness!$A$1:$D$42</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="207">
   <si>
     <t>year</t>
   </si>
@@ -195,6 +203,459 @@
   </si>
   <si>
     <t>note</t>
+  </si>
+  <si>
+    <t>lifesatisfaction_1</t>
+  </si>
+  <si>
+    <t>lifesatisfaction_2</t>
+  </si>
+  <si>
+    <t>jlb505c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jlb505b </t>
+  </si>
+  <si>
+    <t>jlb505a</t>
+  </si>
+  <si>
+    <t>lifesatisfaction_3</t>
+  </si>
+  <si>
+    <t>jlb505d</t>
+  </si>
+  <si>
+    <t>lifesatisfaction_4</t>
+  </si>
+  <si>
+    <t>lifesatisfaction_5</t>
+  </si>
+  <si>
+    <t>jlb505e</t>
+  </si>
+  <si>
+    <t>klb003a</t>
+  </si>
+  <si>
+    <t>klb003b</t>
+  </si>
+  <si>
+    <t>klb003c</t>
+  </si>
+  <si>
+    <t>klb003d</t>
+  </si>
+  <si>
+    <t>klb003e</t>
+  </si>
+  <si>
+    <t>mlb003a</t>
+  </si>
+  <si>
+    <t>llb003a</t>
+  </si>
+  <si>
+    <t>llb003b</t>
+  </si>
+  <si>
+    <t>llb003c</t>
+  </si>
+  <si>
+    <t>llb003d</t>
+  </si>
+  <si>
+    <t>llb003e</t>
+  </si>
+  <si>
+    <t>mlb003b</t>
+  </si>
+  <si>
+    <t>mlb003c</t>
+  </si>
+  <si>
+    <t>mlb003d</t>
+  </si>
+  <si>
+    <t>mlb003e</t>
+  </si>
+  <si>
+    <t>nlb003a</t>
+  </si>
+  <si>
+    <t>nlb003b</t>
+  </si>
+  <si>
+    <t>nlb003c</t>
+  </si>
+  <si>
+    <t>nlb003d</t>
+  </si>
+  <si>
+    <t>nlb003e</t>
+  </si>
+  <si>
+    <t>olb002a</t>
+  </si>
+  <si>
+    <t>olb002b</t>
+  </si>
+  <si>
+    <t>olb002c</t>
+  </si>
+  <si>
+    <t>olb002d</t>
+  </si>
+  <si>
+    <t>olb002e</t>
+  </si>
+  <si>
+    <t>snspouse</t>
+  </si>
+  <si>
+    <t>snchild</t>
+  </si>
+  <si>
+    <t>snfamily</t>
+  </si>
+  <si>
+    <t>snfriends</t>
+  </si>
+  <si>
+    <t>jlb507</t>
+  </si>
+  <si>
+    <t>jlb510</t>
+  </si>
+  <si>
+    <t>jlb514</t>
+  </si>
+  <si>
+    <t>jlb518</t>
+  </si>
+  <si>
+    <t>closespouse</t>
+  </si>
+  <si>
+    <t>closechild</t>
+  </si>
+  <si>
+    <t>closefam</t>
+  </si>
+  <si>
+    <t>closefri</t>
+  </si>
+  <si>
+    <t>mtchild</t>
+  </si>
+  <si>
+    <t>spkchild</t>
+  </si>
+  <si>
+    <t>wrtchild</t>
+  </si>
+  <si>
+    <t>mtfam</t>
+  </si>
+  <si>
+    <t>spkfam</t>
+  </si>
+  <si>
+    <t>wrtfam</t>
+  </si>
+  <si>
+    <t>mtfriend</t>
+  </si>
+  <si>
+    <t>spkfriend</t>
+  </si>
+  <si>
+    <t>wrtfriend</t>
+  </si>
+  <si>
+    <t>ssup1sp</t>
+  </si>
+  <si>
+    <t>ssup2sp</t>
+  </si>
+  <si>
+    <t>ssup3sp</t>
+  </si>
+  <si>
+    <t>ssup5sp</t>
+  </si>
+  <si>
+    <t>jlb509</t>
+  </si>
+  <si>
+    <t>jlb513</t>
+  </si>
+  <si>
+    <t>jlb517</t>
+  </si>
+  <si>
+    <t>jlb521</t>
+  </si>
+  <si>
+    <t>jlb512a</t>
+  </si>
+  <si>
+    <t>jlb512b</t>
+  </si>
+  <si>
+    <t>jlb512c</t>
+  </si>
+  <si>
+    <t>jlb516a</t>
+  </si>
+  <si>
+    <t>jlb516b</t>
+  </si>
+  <si>
+    <t>jlb516c</t>
+  </si>
+  <si>
+    <t>jlb520a</t>
+  </si>
+  <si>
+    <t>jlb520b</t>
+  </si>
+  <si>
+    <t>jlb520c</t>
+  </si>
+  <si>
+    <t>jlb508a</t>
+  </si>
+  <si>
+    <t>jlb508b</t>
+  </si>
+  <si>
+    <t>jlb508c</t>
+  </si>
+  <si>
+    <t>jlb508d</t>
+  </si>
+  <si>
+    <t>jlb508e</t>
+  </si>
+  <si>
+    <t>ssup6sp</t>
+  </si>
+  <si>
+    <t>ssup7sp</t>
+  </si>
+  <si>
+    <t>jlb508f</t>
+  </si>
+  <si>
+    <t>jlb511a</t>
+  </si>
+  <si>
+    <t>ssup1ch</t>
+  </si>
+  <si>
+    <t>jlb511b</t>
+  </si>
+  <si>
+    <t>ssup2ch</t>
+  </si>
+  <si>
+    <t>jlb511c</t>
+  </si>
+  <si>
+    <t>ssup3ch</t>
+  </si>
+  <si>
+    <t>jlb511d</t>
+  </si>
+  <si>
+    <t>ssup5ch</t>
+  </si>
+  <si>
+    <t>jlb511e</t>
+  </si>
+  <si>
+    <t>ssup6ch</t>
+  </si>
+  <si>
+    <t>jlb511f</t>
+  </si>
+  <si>
+    <t>ssup7ch</t>
+  </si>
+  <si>
+    <t>jlb515a</t>
+  </si>
+  <si>
+    <t>ssup1fam</t>
+  </si>
+  <si>
+    <t>jlb515b</t>
+  </si>
+  <si>
+    <t>ssup2fam</t>
+  </si>
+  <si>
+    <t>ssup3fam</t>
+  </si>
+  <si>
+    <t>jlb515c</t>
+  </si>
+  <si>
+    <t>jlb515d</t>
+  </si>
+  <si>
+    <t>ssup5fam</t>
+  </si>
+  <si>
+    <t>jlb515e</t>
+  </si>
+  <si>
+    <t>ssup6fam</t>
+  </si>
+  <si>
+    <t>jlb515f</t>
+  </si>
+  <si>
+    <t>ssup7fam</t>
+  </si>
+  <si>
+    <t>jlb519a</t>
+  </si>
+  <si>
+    <t>ssup1fr</t>
+  </si>
+  <si>
+    <t>jlb519b</t>
+  </si>
+  <si>
+    <t>ssup2fr</t>
+  </si>
+  <si>
+    <t>jlb519c</t>
+  </si>
+  <si>
+    <t>ssup3fr</t>
+  </si>
+  <si>
+    <t>jlb519d</t>
+  </si>
+  <si>
+    <t>ssup5fr</t>
+  </si>
+  <si>
+    <t>jlb519e</t>
+  </si>
+  <si>
+    <t>ssup6fr</t>
+  </si>
+  <si>
+    <t>ssup7fr</t>
+  </si>
+  <si>
+    <t>jlb519f</t>
+  </si>
+  <si>
+    <t>klb004</t>
+  </si>
+  <si>
+    <t>klb007</t>
+  </si>
+  <si>
+    <t>klb011</t>
+  </si>
+  <si>
+    <t>klb015</t>
+  </si>
+  <si>
+    <t>klb006</t>
+  </si>
+  <si>
+    <t>klb010</t>
+  </si>
+  <si>
+    <t>klb014</t>
+  </si>
+  <si>
+    <t>klb018</t>
+  </si>
+  <si>
+    <t>klb009a</t>
+  </si>
+  <si>
+    <t>klb009b</t>
+  </si>
+  <si>
+    <t>klb009c</t>
+  </si>
+  <si>
+    <t>klb013a</t>
+  </si>
+  <si>
+    <t>klb013b</t>
+  </si>
+  <si>
+    <t>klb013c</t>
+  </si>
+  <si>
+    <t>klb017a</t>
+  </si>
+  <si>
+    <t>klb017b</t>
+  </si>
+  <si>
+    <t>klb017c</t>
+  </si>
+  <si>
+    <t>llb004</t>
+  </si>
+  <si>
+    <t>llb007</t>
+  </si>
+  <si>
+    <t>llb011</t>
+  </si>
+  <si>
+    <t>llb015</t>
+  </si>
+  <si>
+    <t>llb006</t>
+  </si>
+  <si>
+    <t>llb010</t>
+  </si>
+  <si>
+    <t>llb014</t>
+  </si>
+  <si>
+    <t>llb018</t>
+  </si>
+  <si>
+    <t>llb009a</t>
+  </si>
+  <si>
+    <t>llb009b</t>
+  </si>
+  <si>
+    <t>llb009c</t>
+  </si>
+  <si>
+    <t>llb013a</t>
+  </si>
+  <si>
+    <t>llb013b</t>
+  </si>
+  <si>
+    <t>llb013c</t>
+  </si>
+  <si>
+    <t>llb017a</t>
+  </si>
+  <si>
+    <t>llb017b</t>
+  </si>
+  <si>
+    <t>llb017c</t>
   </si>
 </sst>
 </file>
@@ -230,8 +691,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,22 +974,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +1006,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2004</v>
       </c>
@@ -558,7 +1020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2004</v>
       </c>
@@ -572,7 +1034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2004</v>
       </c>
@@ -586,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2004</v>
       </c>
@@ -597,7 +1059,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2006</v>
       </c>
@@ -611,7 +1073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2006</v>
       </c>
@@ -625,7 +1087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -639,7 +1101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2008</v>
       </c>
@@ -653,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -667,7 +1129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2008</v>
       </c>
@@ -681,7 +1143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2008</v>
       </c>
@@ -692,7 +1154,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2008</v>
       </c>
@@ -706,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2008</v>
       </c>
@@ -717,7 +1179,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2008</v>
       </c>
@@ -728,7 +1190,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2008</v>
       </c>
@@ -739,7 +1201,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2008</v>
       </c>
@@ -750,7 +1212,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2008</v>
       </c>
@@ -761,7 +1223,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2008</v>
       </c>
@@ -772,7 +1234,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2010</v>
       </c>
@@ -786,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2010</v>
       </c>
@@ -800,7 +1262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2010</v>
       </c>
@@ -814,7 +1276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2010</v>
       </c>
@@ -825,7 +1287,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2010</v>
       </c>
@@ -839,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2010</v>
       </c>
@@ -850,7 +1312,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2010</v>
       </c>
@@ -861,7 +1323,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2010</v>
       </c>
@@ -872,7 +1334,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2010</v>
       </c>
@@ -883,7 +1345,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2010</v>
       </c>
@@ -894,7 +1356,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2010</v>
       </c>
@@ -905,7 +1367,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2012</v>
       </c>
@@ -919,7 +1381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2012</v>
       </c>
@@ -933,7 +1395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2012</v>
       </c>
@@ -947,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2012</v>
       </c>
@@ -958,7 +1420,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2012</v>
       </c>
@@ -972,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2012</v>
       </c>
@@ -983,7 +1445,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2012</v>
       </c>
@@ -994,7 +1456,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2012</v>
       </c>
@@ -1005,7 +1467,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2012</v>
       </c>
@@ -1016,7 +1478,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2012</v>
       </c>
@@ -1027,7 +1489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2012</v>
       </c>
@@ -1038,7 +1500,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A1:D42">
     <filterColumn colId="2">
@@ -1052,4 +1514,1220 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView zoomScale="110" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2004</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2004</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2004</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2006</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2006</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2006</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2006</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2006</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2008</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2008</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2008</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2008</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2008</v>
+      </c>
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2010</v>
+      </c>
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2010</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2010</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2010</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2010</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2012</v>
+      </c>
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2012</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2012</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2012</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2012</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2014</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2014</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2014</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2014</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2014</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:A76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2004</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2004</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2004</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2004</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2004</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2004</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2004</v>
+      </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2004</v>
+      </c>
+      <c r="B11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2004</v>
+      </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2004</v>
+      </c>
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2004</v>
+      </c>
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2004</v>
+      </c>
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2004</v>
+      </c>
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2004</v>
+      </c>
+      <c r="B17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2004</v>
+      </c>
+      <c r="B18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2004</v>
+      </c>
+      <c r="B19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2004</v>
+      </c>
+      <c r="B20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2004</v>
+      </c>
+      <c r="B21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2004</v>
+      </c>
+      <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2004</v>
+      </c>
+      <c r="B23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2004</v>
+      </c>
+      <c r="B24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2004</v>
+      </c>
+      <c r="B25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2004</v>
+      </c>
+      <c r="B26" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2004</v>
+      </c>
+      <c r="B27" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2004</v>
+      </c>
+      <c r="B28" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2004</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C29" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2004</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2004</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2004</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2004</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2004</v>
+      </c>
+      <c r="B34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2004</v>
+      </c>
+      <c r="B35" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2004</v>
+      </c>
+      <c r="B36" t="s">
+        <v>159</v>
+      </c>
+      <c r="C36" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2004</v>
+      </c>
+      <c r="B37" t="s">
+        <v>161</v>
+      </c>
+      <c r="C37" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2004</v>
+      </c>
+      <c r="B38" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2004</v>
+      </c>
+      <c r="B39" t="s">
+        <v>165</v>
+      </c>
+      <c r="C39" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2004</v>
+      </c>
+      <c r="B40" t="s">
+        <v>167</v>
+      </c>
+      <c r="C40" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2004</v>
+      </c>
+      <c r="B41" t="s">
+        <v>169</v>
+      </c>
+      <c r="C41" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2004</v>
+      </c>
+      <c r="B42" t="s">
+        <v>172</v>
+      </c>
+      <c r="C42" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2006</v>
+      </c>
+      <c r="B43" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2006</v>
+      </c>
+      <c r="B44" t="s">
+        <v>174</v>
+      </c>
+      <c r="C44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2006</v>
+      </c>
+      <c r="B45" t="s">
+        <v>175</v>
+      </c>
+      <c r="C45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2006</v>
+      </c>
+      <c r="B46" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2006</v>
+      </c>
+      <c r="B47" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2006</v>
+      </c>
+      <c r="B48" t="s">
+        <v>178</v>
+      </c>
+      <c r="C48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2006</v>
+      </c>
+      <c r="B49" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2006</v>
+      </c>
+      <c r="B50" t="s">
+        <v>180</v>
+      </c>
+      <c r="C50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2006</v>
+      </c>
+      <c r="B51" t="s">
+        <v>181</v>
+      </c>
+      <c r="C51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2006</v>
+      </c>
+      <c r="B52" t="s">
+        <v>182</v>
+      </c>
+      <c r="C52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2006</v>
+      </c>
+      <c r="B53" t="s">
+        <v>183</v>
+      </c>
+      <c r="C53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2006</v>
+      </c>
+      <c r="B54" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2006</v>
+      </c>
+      <c r="B55" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>2006</v>
+      </c>
+      <c r="B56" t="s">
+        <v>186</v>
+      </c>
+      <c r="C56" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>2006</v>
+      </c>
+      <c r="B57" t="s">
+        <v>187</v>
+      </c>
+      <c r="C57" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2006</v>
+      </c>
+      <c r="B58" t="s">
+        <v>188</v>
+      </c>
+      <c r="C58" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>2006</v>
+      </c>
+      <c r="B59" t="s">
+        <v>189</v>
+      </c>
+      <c r="C59" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>2008</v>
+      </c>
+      <c r="B60" t="s">
+        <v>190</v>
+      </c>
+      <c r="C60" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>2008</v>
+      </c>
+      <c r="B61" t="s">
+        <v>191</v>
+      </c>
+      <c r="C61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2008</v>
+      </c>
+      <c r="B62" t="s">
+        <v>192</v>
+      </c>
+      <c r="C62" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2008</v>
+      </c>
+      <c r="B63" t="s">
+        <v>193</v>
+      </c>
+      <c r="C63" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>2008</v>
+      </c>
+      <c r="B64" t="s">
+        <v>194</v>
+      </c>
+      <c r="C64" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>2008</v>
+      </c>
+      <c r="B65" t="s">
+        <v>195</v>
+      </c>
+      <c r="C65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>2008</v>
+      </c>
+      <c r="B66" t="s">
+        <v>196</v>
+      </c>
+      <c r="C66" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>2008</v>
+      </c>
+      <c r="B67" t="s">
+        <v>197</v>
+      </c>
+      <c r="C67" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>2008</v>
+      </c>
+      <c r="B68" t="s">
+        <v>198</v>
+      </c>
+      <c r="C68" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>2008</v>
+      </c>
+      <c r="B69" t="s">
+        <v>199</v>
+      </c>
+      <c r="C69" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>2008</v>
+      </c>
+      <c r="B70" t="s">
+        <v>200</v>
+      </c>
+      <c r="C70" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>2008</v>
+      </c>
+      <c r="B71" t="s">
+        <v>201</v>
+      </c>
+      <c r="C71" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>2008</v>
+      </c>
+      <c r="B72" t="s">
+        <v>202</v>
+      </c>
+      <c r="C72" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>2008</v>
+      </c>
+      <c r="B73" t="s">
+        <v>203</v>
+      </c>
+      <c r="C73" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>2008</v>
+      </c>
+      <c r="B74" t="s">
+        <v>204</v>
+      </c>
+      <c r="C74" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>2008</v>
+      </c>
+      <c r="B75" t="s">
+        <v>205</v>
+      </c>
+      <c r="C75" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>2008</v>
+      </c>
+      <c r="B76" t="s">
+        <v>206</v>
+      </c>
+      <c r="C76" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Renaming rules demographics added
</commit_message>
<xml_diff>
--- a/data-phi-free/raw/renaming-rules/renaming-rules.xlsx
+++ b/data-phi-free/raw/renaming-rules/renaming-rules.xlsx
@@ -9,21 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20220" activeTab="1"/>
+    <workbookView xWindow="33600" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="loneliness" sheetId="1" r:id="rId1"/>
     <sheet name="lifesatisfaction" sheetId="2" r:id="rId2"/>
     <sheet name="socialnetwork" sheetId="3" r:id="rId3"/>
     <sheet name="activity" sheetId="4" r:id="rId4"/>
-    <sheet name="socialsupport" sheetId="5" r:id="rId5"/>
-    <sheet name="wellbeing" sheetId="6" r:id="rId6"/>
-    <sheet name="selfratedmemory" sheetId="7" r:id="rId7"/>
-    <sheet name="wordlist" sheetId="8" r:id="rId8"/>
-    <sheet name="mentalstatus" sheetId="10" r:id="rId9"/>
-    <sheet name="vocabulary" sheetId="9" r:id="rId10"/>
+    <sheet name="demographics" sheetId="11" r:id="rId5"/>
+    <sheet name="socialsupport" sheetId="5" r:id="rId6"/>
+    <sheet name="wellbeing" sheetId="6" r:id="rId7"/>
+    <sheet name="selfratedmemory" sheetId="7" r:id="rId8"/>
+    <sheet name="wordlist" sheetId="8" r:id="rId9"/>
+    <sheet name="mentalstatus" sheetId="10" r:id="rId10"/>
+    <sheet name="vocabulary" sheetId="9" r:id="rId11"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">activity!$A$1:$E$90</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">loneliness!$A$1:$D$42</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="917">
   <si>
     <t>year</t>
   </si>
@@ -2169,6 +2171,630 @@
   </si>
   <si>
     <t>od167</t>
+  </si>
+  <si>
+    <t>interview_yr</t>
+  </si>
+  <si>
+    <t>nursing_home_mth</t>
+  </si>
+  <si>
+    <t>interview_mth</t>
+  </si>
+  <si>
+    <t>nursing_home_yr</t>
+  </si>
+  <si>
+    <t>1st_marriage_mth</t>
+  </si>
+  <si>
+    <t>1st_marriage_yr</t>
+  </si>
+  <si>
+    <t>2nd_marriage_mth</t>
+  </si>
+  <si>
+    <t>2nd_marriage_yr</t>
+  </si>
+  <si>
+    <t>3rd_marriage_mth</t>
+  </si>
+  <si>
+    <t>3rd_marriage_yr</t>
+  </si>
+  <si>
+    <t>4th_marriage_mth</t>
+  </si>
+  <si>
+    <t>4th_marriage_yr</t>
+  </si>
+  <si>
+    <t>btw_wave_marriage_mth</t>
+  </si>
+  <si>
+    <t>btw_wave_marriage_yr</t>
+  </si>
+  <si>
+    <t>proxy_interview</t>
+  </si>
+  <si>
+    <t>1 means self interview, 2 means proxy interview with spouse as respondent, 3 is proxy interview non-spouse as respondent, 4 is proxy interview spouse is respondent but the spouses no longer living together</t>
+  </si>
+  <si>
+    <t>proxy_ratiing_cognitive</t>
+  </si>
+  <si>
+    <t>interview_language</t>
+  </si>
+  <si>
+    <t>1 is English, 2 is Spanish</t>
+  </si>
+  <si>
+    <t>age_at_visit</t>
+  </si>
+  <si>
+    <t>nursing_home</t>
+  </si>
+  <si>
+    <t>us_born</t>
+  </si>
+  <si>
+    <t>arrive_us_year</t>
+  </si>
+  <si>
+    <t>ses</t>
+  </si>
+  <si>
+    <t>religion</t>
+  </si>
+  <si>
+    <t>religious_service</t>
+  </si>
+  <si>
+    <t>religion_importance</t>
+  </si>
+  <si>
+    <t>english_household</t>
+  </si>
+  <si>
+    <t>number_marriages</t>
+  </si>
+  <si>
+    <t>married</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>hispanic</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>ka500</t>
+  </si>
+  <si>
+    <t>ka501</t>
+  </si>
+  <si>
+    <t>ka065</t>
+  </si>
+  <si>
+    <t>ka066</t>
+  </si>
+  <si>
+    <t>kb066.1</t>
+  </si>
+  <si>
+    <t>kb067.1</t>
+  </si>
+  <si>
+    <t>kb066.2</t>
+  </si>
+  <si>
+    <t>kb067.2</t>
+  </si>
+  <si>
+    <t>kb066.3</t>
+  </si>
+  <si>
+    <t>kb067.3</t>
+  </si>
+  <si>
+    <t>kb066.4</t>
+  </si>
+  <si>
+    <t>kb067.4</t>
+  </si>
+  <si>
+    <t>kb056</t>
+  </si>
+  <si>
+    <t>kb057</t>
+  </si>
+  <si>
+    <t>ka009</t>
+  </si>
+  <si>
+    <t>ka011</t>
+  </si>
+  <si>
+    <t>ka012</t>
+  </si>
+  <si>
+    <t>ka019</t>
+  </si>
+  <si>
+    <t>ka028</t>
+  </si>
+  <si>
+    <t>kb002</t>
+  </si>
+  <si>
+    <t>kb006</t>
+  </si>
+  <si>
+    <t>kb020</t>
+  </si>
+  <si>
+    <t>kb050</t>
+  </si>
+  <si>
+    <t>kb082</t>
+  </si>
+  <si>
+    <t>kb053</t>
+  </si>
+  <si>
+    <t>kb054</t>
+  </si>
+  <si>
+    <t>kb065</t>
+  </si>
+  <si>
+    <t>kb063</t>
+  </si>
+  <si>
+    <t>kx060_r</t>
+  </si>
+  <si>
+    <t>jx060_r</t>
+  </si>
+  <si>
+    <t>ja500</t>
+  </si>
+  <si>
+    <t>ja501</t>
+  </si>
+  <si>
+    <t>ja065</t>
+  </si>
+  <si>
+    <t>ja066</t>
+  </si>
+  <si>
+    <t>jb066.1</t>
+  </si>
+  <si>
+    <t>jb067.1</t>
+  </si>
+  <si>
+    <t>jb066.2</t>
+  </si>
+  <si>
+    <t>jb067.2</t>
+  </si>
+  <si>
+    <t>jb066.3</t>
+  </si>
+  <si>
+    <t>jb067.3</t>
+  </si>
+  <si>
+    <t>jb066.4</t>
+  </si>
+  <si>
+    <t>jb067.4</t>
+  </si>
+  <si>
+    <t>jb056</t>
+  </si>
+  <si>
+    <t>jb057</t>
+  </si>
+  <si>
+    <t>ja009</t>
+  </si>
+  <si>
+    <t>ja011</t>
+  </si>
+  <si>
+    <t>ja012</t>
+  </si>
+  <si>
+    <t>ja019</t>
+  </si>
+  <si>
+    <t>ja028</t>
+  </si>
+  <si>
+    <t>jb002</t>
+  </si>
+  <si>
+    <t>jb006</t>
+  </si>
+  <si>
+    <t>jb020</t>
+  </si>
+  <si>
+    <t>jb050</t>
+  </si>
+  <si>
+    <t>jb082</t>
+  </si>
+  <si>
+    <t>jb053</t>
+  </si>
+  <si>
+    <t>jb054</t>
+  </si>
+  <si>
+    <t>jb065</t>
+  </si>
+  <si>
+    <t>jb063</t>
+  </si>
+  <si>
+    <t>la500</t>
+  </si>
+  <si>
+    <t>la501</t>
+  </si>
+  <si>
+    <t>la065</t>
+  </si>
+  <si>
+    <t>la066</t>
+  </si>
+  <si>
+    <t>lb066.1</t>
+  </si>
+  <si>
+    <t>lb067.1</t>
+  </si>
+  <si>
+    <t>lb066.2</t>
+  </si>
+  <si>
+    <t>lb067.2</t>
+  </si>
+  <si>
+    <t>lb066.3</t>
+  </si>
+  <si>
+    <t>lb067.3</t>
+  </si>
+  <si>
+    <t>lb066.4</t>
+  </si>
+  <si>
+    <t>lb067.4</t>
+  </si>
+  <si>
+    <t>lb056</t>
+  </si>
+  <si>
+    <t>lb057</t>
+  </si>
+  <si>
+    <t>la009</t>
+  </si>
+  <si>
+    <t>la011</t>
+  </si>
+  <si>
+    <t>la012</t>
+  </si>
+  <si>
+    <t>la019</t>
+  </si>
+  <si>
+    <t>la028</t>
+  </si>
+  <si>
+    <t>lb002</t>
+  </si>
+  <si>
+    <t>lb006</t>
+  </si>
+  <si>
+    <t>lb020</t>
+  </si>
+  <si>
+    <t>lb050</t>
+  </si>
+  <si>
+    <t>lb082</t>
+  </si>
+  <si>
+    <t>lb053</t>
+  </si>
+  <si>
+    <t>lb054</t>
+  </si>
+  <si>
+    <t>lb065</t>
+  </si>
+  <si>
+    <t>lb063</t>
+  </si>
+  <si>
+    <t>lx060_r</t>
+  </si>
+  <si>
+    <t>ma500</t>
+  </si>
+  <si>
+    <t>ma501</t>
+  </si>
+  <si>
+    <t>ma065</t>
+  </si>
+  <si>
+    <t>ma066</t>
+  </si>
+  <si>
+    <t>mb066.1</t>
+  </si>
+  <si>
+    <t>mb067.1</t>
+  </si>
+  <si>
+    <t>mb066.2</t>
+  </si>
+  <si>
+    <t>mb067.2</t>
+  </si>
+  <si>
+    <t>mb066.3</t>
+  </si>
+  <si>
+    <t>mb067.3</t>
+  </si>
+  <si>
+    <t>mb066.4</t>
+  </si>
+  <si>
+    <t>mb067.4</t>
+  </si>
+  <si>
+    <t>mb056</t>
+  </si>
+  <si>
+    <t>mb057</t>
+  </si>
+  <si>
+    <t>ma009</t>
+  </si>
+  <si>
+    <t>ma011</t>
+  </si>
+  <si>
+    <t>ma012</t>
+  </si>
+  <si>
+    <t>ma019</t>
+  </si>
+  <si>
+    <t>ma028</t>
+  </si>
+  <si>
+    <t>mb002</t>
+  </si>
+  <si>
+    <t>mb006</t>
+  </si>
+  <si>
+    <t>mb020</t>
+  </si>
+  <si>
+    <t>mb050</t>
+  </si>
+  <si>
+    <t>mb082</t>
+  </si>
+  <si>
+    <t>mb053</t>
+  </si>
+  <si>
+    <t>mb054</t>
+  </si>
+  <si>
+    <t>mb065</t>
+  </si>
+  <si>
+    <t>mb063</t>
+  </si>
+  <si>
+    <t>mx060_r</t>
+  </si>
+  <si>
+    <t>na500</t>
+  </si>
+  <si>
+    <t>na501</t>
+  </si>
+  <si>
+    <t>na065</t>
+  </si>
+  <si>
+    <t>na066</t>
+  </si>
+  <si>
+    <t>nb066.1</t>
+  </si>
+  <si>
+    <t>nb067.1</t>
+  </si>
+  <si>
+    <t>nb066.2</t>
+  </si>
+  <si>
+    <t>nb067.2</t>
+  </si>
+  <si>
+    <t>nb066.3</t>
+  </si>
+  <si>
+    <t>nb067.3</t>
+  </si>
+  <si>
+    <t>nb066.4</t>
+  </si>
+  <si>
+    <t>nb067.4</t>
+  </si>
+  <si>
+    <t>nb056</t>
+  </si>
+  <si>
+    <t>nb057</t>
+  </si>
+  <si>
+    <t>na009</t>
+  </si>
+  <si>
+    <t>na011</t>
+  </si>
+  <si>
+    <t>na012</t>
+  </si>
+  <si>
+    <t>na019</t>
+  </si>
+  <si>
+    <t>na028</t>
+  </si>
+  <si>
+    <t>nb002</t>
+  </si>
+  <si>
+    <t>nb006</t>
+  </si>
+  <si>
+    <t>nb020</t>
+  </si>
+  <si>
+    <t>nb050</t>
+  </si>
+  <si>
+    <t>nb082</t>
+  </si>
+  <si>
+    <t>nb053</t>
+  </si>
+  <si>
+    <t>nb054</t>
+  </si>
+  <si>
+    <t>nb065</t>
+  </si>
+  <si>
+    <t>nb063</t>
+  </si>
+  <si>
+    <t>nx060_r</t>
+  </si>
+  <si>
+    <t>oa500</t>
+  </si>
+  <si>
+    <t>oa501</t>
+  </si>
+  <si>
+    <t>oa065</t>
+  </si>
+  <si>
+    <t>oa066</t>
+  </si>
+  <si>
+    <t>ob066.1</t>
+  </si>
+  <si>
+    <t>ob067.1</t>
+  </si>
+  <si>
+    <t>ob066.2</t>
+  </si>
+  <si>
+    <t>ob067.2</t>
+  </si>
+  <si>
+    <t>ob066.3</t>
+  </si>
+  <si>
+    <t>ob067.3</t>
+  </si>
+  <si>
+    <t>ob066.4</t>
+  </si>
+  <si>
+    <t>ob067.4</t>
+  </si>
+  <si>
+    <t>ob056</t>
+  </si>
+  <si>
+    <t>ob057</t>
+  </si>
+  <si>
+    <t>oa009</t>
+  </si>
+  <si>
+    <t>oa011</t>
+  </si>
+  <si>
+    <t>oa012</t>
+  </si>
+  <si>
+    <t>oa019</t>
+  </si>
+  <si>
+    <t>oa028</t>
+  </si>
+  <si>
+    <t>ob002</t>
+  </si>
+  <si>
+    <t>ob006</t>
+  </si>
+  <si>
+    <t>ob020</t>
+  </si>
+  <si>
+    <t>ob050</t>
+  </si>
+  <si>
+    <t>ob082</t>
+  </si>
+  <si>
+    <t>ob053</t>
+  </si>
+  <si>
+    <t>ob054</t>
+  </si>
+  <si>
+    <t>ob065</t>
+  </si>
+  <si>
+    <t>ob063</t>
+  </si>
+  <si>
+    <t>ox060_r</t>
   </si>
 </sst>
 </file>
@@ -3032,6 +3658,566 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2004</v>
+      </c>
+      <c r="B2" t="s">
+        <v>614</v>
+      </c>
+      <c r="C2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2004</v>
+      </c>
+      <c r="B3" t="s">
+        <v>615</v>
+      </c>
+      <c r="C3" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2004</v>
+      </c>
+      <c r="B4" t="s">
+        <v>616</v>
+      </c>
+      <c r="C4" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>617</v>
+      </c>
+      <c r="C5" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>618</v>
+      </c>
+      <c r="C6" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2004</v>
+      </c>
+      <c r="B7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C7" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2004</v>
+      </c>
+      <c r="B8" t="s">
+        <v>620</v>
+      </c>
+      <c r="C8" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2004</v>
+      </c>
+      <c r="B9" t="s">
+        <v>621</v>
+      </c>
+      <c r="C9" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2006</v>
+      </c>
+      <c r="B10" t="s">
+        <v>630</v>
+      </c>
+      <c r="C10" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2006</v>
+      </c>
+      <c r="B11" t="s">
+        <v>631</v>
+      </c>
+      <c r="C11" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2006</v>
+      </c>
+      <c r="B12" t="s">
+        <v>632</v>
+      </c>
+      <c r="C12" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2006</v>
+      </c>
+      <c r="B13" t="s">
+        <v>633</v>
+      </c>
+      <c r="C13" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2006</v>
+      </c>
+      <c r="B14" t="s">
+        <v>634</v>
+      </c>
+      <c r="C14" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2006</v>
+      </c>
+      <c r="B15" t="s">
+        <v>635</v>
+      </c>
+      <c r="C15" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2006</v>
+      </c>
+      <c r="B16" t="s">
+        <v>636</v>
+      </c>
+      <c r="C16" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2006</v>
+      </c>
+      <c r="B17" t="s">
+        <v>637</v>
+      </c>
+      <c r="C17" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2008</v>
+      </c>
+      <c r="B18" t="s">
+        <v>638</v>
+      </c>
+      <c r="C18" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2008</v>
+      </c>
+      <c r="B19" t="s">
+        <v>639</v>
+      </c>
+      <c r="C19" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2008</v>
+      </c>
+      <c r="B20" t="s">
+        <v>640</v>
+      </c>
+      <c r="C20" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2008</v>
+      </c>
+      <c r="B21" t="s">
+        <v>641</v>
+      </c>
+      <c r="C21" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2008</v>
+      </c>
+      <c r="B22" t="s">
+        <v>642</v>
+      </c>
+      <c r="C22" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2008</v>
+      </c>
+      <c r="B23" t="s">
+        <v>643</v>
+      </c>
+      <c r="C23" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2008</v>
+      </c>
+      <c r="B24" t="s">
+        <v>644</v>
+      </c>
+      <c r="C24" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2008</v>
+      </c>
+      <c r="B25" t="s">
+        <v>645</v>
+      </c>
+      <c r="C25" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2010</v>
+      </c>
+      <c r="B26" t="s">
+        <v>646</v>
+      </c>
+      <c r="C26" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2010</v>
+      </c>
+      <c r="B27" t="s">
+        <v>647</v>
+      </c>
+      <c r="C27" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2010</v>
+      </c>
+      <c r="B28" t="s">
+        <v>648</v>
+      </c>
+      <c r="C28" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2010</v>
+      </c>
+      <c r="B29" t="s">
+        <v>649</v>
+      </c>
+      <c r="C29" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2010</v>
+      </c>
+      <c r="B30" t="s">
+        <v>650</v>
+      </c>
+      <c r="C30" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2010</v>
+      </c>
+      <c r="B31" t="s">
+        <v>651</v>
+      </c>
+      <c r="C31" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2010</v>
+      </c>
+      <c r="B32" t="s">
+        <v>652</v>
+      </c>
+      <c r="C32" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2010</v>
+      </c>
+      <c r="B33" t="s">
+        <v>653</v>
+      </c>
+      <c r="C33" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2012</v>
+      </c>
+      <c r="B34" t="s">
+        <v>654</v>
+      </c>
+      <c r="C34" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2012</v>
+      </c>
+      <c r="B35" t="s">
+        <v>655</v>
+      </c>
+      <c r="C35" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2012</v>
+      </c>
+      <c r="B36" t="s">
+        <v>656</v>
+      </c>
+      <c r="C36" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2012</v>
+      </c>
+      <c r="B37" t="s">
+        <v>657</v>
+      </c>
+      <c r="C37" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2012</v>
+      </c>
+      <c r="B38" t="s">
+        <v>658</v>
+      </c>
+      <c r="C38" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2012</v>
+      </c>
+      <c r="B39" t="s">
+        <v>659</v>
+      </c>
+      <c r="C39" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2012</v>
+      </c>
+      <c r="B40" t="s">
+        <v>660</v>
+      </c>
+      <c r="C40" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2012</v>
+      </c>
+      <c r="B41" t="s">
+        <v>661</v>
+      </c>
+      <c r="C41" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2014</v>
+      </c>
+      <c r="B42" t="s">
+        <v>662</v>
+      </c>
+      <c r="C42" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2014</v>
+      </c>
+      <c r="B43" t="s">
+        <v>663</v>
+      </c>
+      <c r="C43" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2014</v>
+      </c>
+      <c r="B44" t="s">
+        <v>664</v>
+      </c>
+      <c r="C44" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2014</v>
+      </c>
+      <c r="B45" t="s">
+        <v>665</v>
+      </c>
+      <c r="C45" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2014</v>
+      </c>
+      <c r="B46" t="s">
+        <v>666</v>
+      </c>
+      <c r="C46" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2014</v>
+      </c>
+      <c r="B47" t="s">
+        <v>667</v>
+      </c>
+      <c r="C47" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2014</v>
+      </c>
+      <c r="B48" t="s">
+        <v>668</v>
+      </c>
+      <c r="C48" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2014</v>
+      </c>
+      <c r="B49" t="s">
+        <v>669</v>
+      </c>
+      <c r="C49" t="s">
+        <v>629</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3462,8 +4648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView zoomScale="110" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5055,8 +6241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6067,11 +7253,2162 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E90"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E193"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2004</v>
+      </c>
+      <c r="B2" t="s">
+        <v>773</v>
+      </c>
+      <c r="C2" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2004</v>
+      </c>
+      <c r="B3" t="s">
+        <v>774</v>
+      </c>
+      <c r="C3" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2004</v>
+      </c>
+      <c r="B4" t="s">
+        <v>775</v>
+      </c>
+      <c r="C4" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>776</v>
+      </c>
+      <c r="C5" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>777</v>
+      </c>
+      <c r="C6" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2004</v>
+      </c>
+      <c r="B7" t="s">
+        <v>778</v>
+      </c>
+      <c r="C7" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2004</v>
+      </c>
+      <c r="B8" t="s">
+        <v>779</v>
+      </c>
+      <c r="C8" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2004</v>
+      </c>
+      <c r="B9" t="s">
+        <v>780</v>
+      </c>
+      <c r="C9" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2004</v>
+      </c>
+      <c r="B10" t="s">
+        <v>781</v>
+      </c>
+      <c r="C10" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2004</v>
+      </c>
+      <c r="B11" t="s">
+        <v>782</v>
+      </c>
+      <c r="C11" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2004</v>
+      </c>
+      <c r="B12" t="s">
+        <v>783</v>
+      </c>
+      <c r="C12" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2004</v>
+      </c>
+      <c r="B13" t="s">
+        <v>784</v>
+      </c>
+      <c r="C13" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2004</v>
+      </c>
+      <c r="B14" t="s">
+        <v>785</v>
+      </c>
+      <c r="C14" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2004</v>
+      </c>
+      <c r="B15" t="s">
+        <v>786</v>
+      </c>
+      <c r="C15" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2004</v>
+      </c>
+      <c r="B16" t="s">
+        <v>787</v>
+      </c>
+      <c r="C16" t="s">
+        <v>723</v>
+      </c>
+      <c r="E16" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2004</v>
+      </c>
+      <c r="B17" t="s">
+        <v>788</v>
+      </c>
+      <c r="C17" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2004</v>
+      </c>
+      <c r="B18" t="s">
+        <v>789</v>
+      </c>
+      <c r="C18" t="s">
+        <v>726</v>
+      </c>
+      <c r="E18" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2004</v>
+      </c>
+      <c r="B19" t="s">
+        <v>790</v>
+      </c>
+      <c r="C19" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2004</v>
+      </c>
+      <c r="B20" t="s">
+        <v>791</v>
+      </c>
+      <c r="C20" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2004</v>
+      </c>
+      <c r="B21" t="s">
+        <v>792</v>
+      </c>
+      <c r="C21" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2004</v>
+      </c>
+      <c r="B22" t="s">
+        <v>793</v>
+      </c>
+      <c r="C22" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2004</v>
+      </c>
+      <c r="B23" t="s">
+        <v>794</v>
+      </c>
+      <c r="C23" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2004</v>
+      </c>
+      <c r="B24" t="s">
+        <v>795</v>
+      </c>
+      <c r="C24" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2004</v>
+      </c>
+      <c r="B25" t="s">
+        <v>796</v>
+      </c>
+      <c r="C25" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2004</v>
+      </c>
+      <c r="B26" t="s">
+        <v>797</v>
+      </c>
+      <c r="C26" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2004</v>
+      </c>
+      <c r="B27" t="s">
+        <v>798</v>
+      </c>
+      <c r="C27" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2004</v>
+      </c>
+      <c r="B28" t="s">
+        <v>799</v>
+      </c>
+      <c r="C28" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2004</v>
+      </c>
+      <c r="B29" t="s">
+        <v>800</v>
+      </c>
+      <c r="C29" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2004</v>
+      </c>
+      <c r="B30" t="s">
+        <v>772</v>
+      </c>
+      <c r="C30" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2004</v>
+      </c>
+      <c r="B31" t="s">
+        <v>740</v>
+      </c>
+      <c r="C31" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2004</v>
+      </c>
+      <c r="B32" t="s">
+        <v>741</v>
+      </c>
+      <c r="C32" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2004</v>
+      </c>
+      <c r="B33" t="s">
+        <v>742</v>
+      </c>
+      <c r="C33" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2006</v>
+      </c>
+      <c r="B34" t="s">
+        <v>743</v>
+      </c>
+      <c r="C34" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2006</v>
+      </c>
+      <c r="B35" t="s">
+        <v>744</v>
+      </c>
+      <c r="C35" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2006</v>
+      </c>
+      <c r="B36" t="s">
+        <v>745</v>
+      </c>
+      <c r="C36" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2006</v>
+      </c>
+      <c r="B37" t="s">
+        <v>746</v>
+      </c>
+      <c r="C37" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2006</v>
+      </c>
+      <c r="B38" t="s">
+        <v>747</v>
+      </c>
+      <c r="C38" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2006</v>
+      </c>
+      <c r="B39" t="s">
+        <v>748</v>
+      </c>
+      <c r="C39" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2006</v>
+      </c>
+      <c r="B40" t="s">
+        <v>749</v>
+      </c>
+      <c r="C40" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2006</v>
+      </c>
+      <c r="B41" t="s">
+        <v>750</v>
+      </c>
+      <c r="C41" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2006</v>
+      </c>
+      <c r="B42" t="s">
+        <v>751</v>
+      </c>
+      <c r="C42" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2006</v>
+      </c>
+      <c r="B43" t="s">
+        <v>752</v>
+      </c>
+      <c r="C43" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2006</v>
+      </c>
+      <c r="B44" t="s">
+        <v>753</v>
+      </c>
+      <c r="C44" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2006</v>
+      </c>
+      <c r="B45" t="s">
+        <v>754</v>
+      </c>
+      <c r="C45" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2006</v>
+      </c>
+      <c r="B46" t="s">
+        <v>755</v>
+      </c>
+      <c r="C46" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2006</v>
+      </c>
+      <c r="B47" t="s">
+        <v>756</v>
+      </c>
+      <c r="C47" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2006</v>
+      </c>
+      <c r="B48" t="s">
+        <v>757</v>
+      </c>
+      <c r="C48" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2006</v>
+      </c>
+      <c r="B49" t="s">
+        <v>758</v>
+      </c>
+      <c r="C49" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2006</v>
+      </c>
+      <c r="B50" t="s">
+        <v>759</v>
+      </c>
+      <c r="C50" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2006</v>
+      </c>
+      <c r="B51" t="s">
+        <v>760</v>
+      </c>
+      <c r="C51" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2006</v>
+      </c>
+      <c r="B52" t="s">
+        <v>761</v>
+      </c>
+      <c r="C52" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2006</v>
+      </c>
+      <c r="B53" t="s">
+        <v>762</v>
+      </c>
+      <c r="C53" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2006</v>
+      </c>
+      <c r="B54" t="s">
+        <v>763</v>
+      </c>
+      <c r="C54" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2006</v>
+      </c>
+      <c r="B55" t="s">
+        <v>764</v>
+      </c>
+      <c r="C55" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>2006</v>
+      </c>
+      <c r="B56" t="s">
+        <v>765</v>
+      </c>
+      <c r="C56" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>2006</v>
+      </c>
+      <c r="B57" t="s">
+        <v>766</v>
+      </c>
+      <c r="C57" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2006</v>
+      </c>
+      <c r="B58" t="s">
+        <v>767</v>
+      </c>
+      <c r="C58" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>2006</v>
+      </c>
+      <c r="B59" t="s">
+        <v>768</v>
+      </c>
+      <c r="C59" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>2006</v>
+      </c>
+      <c r="B60" t="s">
+        <v>769</v>
+      </c>
+      <c r="C60" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>2006</v>
+      </c>
+      <c r="B61" t="s">
+        <v>770</v>
+      </c>
+      <c r="C61" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2006</v>
+      </c>
+      <c r="B62" t="s">
+        <v>771</v>
+      </c>
+      <c r="C62" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2006</v>
+      </c>
+      <c r="B63" t="s">
+        <v>740</v>
+      </c>
+      <c r="C63" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>2006</v>
+      </c>
+      <c r="B64" t="s">
+        <v>741</v>
+      </c>
+      <c r="C64" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>2006</v>
+      </c>
+      <c r="B65" t="s">
+        <v>742</v>
+      </c>
+      <c r="C65" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>2008</v>
+      </c>
+      <c r="B66" t="s">
+        <v>801</v>
+      </c>
+      <c r="C66" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>2008</v>
+      </c>
+      <c r="B67" t="s">
+        <v>802</v>
+      </c>
+      <c r="C67" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>2008</v>
+      </c>
+      <c r="B68" t="s">
+        <v>803</v>
+      </c>
+      <c r="C68" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>2008</v>
+      </c>
+      <c r="B69" t="s">
+        <v>804</v>
+      </c>
+      <c r="C69" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>2008</v>
+      </c>
+      <c r="B70" t="s">
+        <v>805</v>
+      </c>
+      <c r="C70" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>2008</v>
+      </c>
+      <c r="B71" t="s">
+        <v>806</v>
+      </c>
+      <c r="C71" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>2008</v>
+      </c>
+      <c r="B72" t="s">
+        <v>807</v>
+      </c>
+      <c r="C72" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>2008</v>
+      </c>
+      <c r="B73" t="s">
+        <v>808</v>
+      </c>
+      <c r="C73" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>2008</v>
+      </c>
+      <c r="B74" t="s">
+        <v>809</v>
+      </c>
+      <c r="C74" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>2008</v>
+      </c>
+      <c r="B75" t="s">
+        <v>810</v>
+      </c>
+      <c r="C75" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>2008</v>
+      </c>
+      <c r="B76" t="s">
+        <v>811</v>
+      </c>
+      <c r="C76" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>2008</v>
+      </c>
+      <c r="B77" t="s">
+        <v>812</v>
+      </c>
+      <c r="C77" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>2008</v>
+      </c>
+      <c r="B78" t="s">
+        <v>813</v>
+      </c>
+      <c r="C78" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>2008</v>
+      </c>
+      <c r="B79" t="s">
+        <v>814</v>
+      </c>
+      <c r="C79" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>2008</v>
+      </c>
+      <c r="B80" t="s">
+        <v>815</v>
+      </c>
+      <c r="C80" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>2008</v>
+      </c>
+      <c r="B81" t="s">
+        <v>816</v>
+      </c>
+      <c r="C81" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>2008</v>
+      </c>
+      <c r="B82" t="s">
+        <v>817</v>
+      </c>
+      <c r="C82" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>2008</v>
+      </c>
+      <c r="B83" t="s">
+        <v>818</v>
+      </c>
+      <c r="C83" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>2008</v>
+      </c>
+      <c r="B84" t="s">
+        <v>819</v>
+      </c>
+      <c r="C84" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>2008</v>
+      </c>
+      <c r="B85" t="s">
+        <v>820</v>
+      </c>
+      <c r="C85" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>2008</v>
+      </c>
+      <c r="B86" t="s">
+        <v>821</v>
+      </c>
+      <c r="C86" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>2008</v>
+      </c>
+      <c r="B87" t="s">
+        <v>822</v>
+      </c>
+      <c r="C87" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>2008</v>
+      </c>
+      <c r="B88" t="s">
+        <v>823</v>
+      </c>
+      <c r="C88" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>2008</v>
+      </c>
+      <c r="B89" t="s">
+        <v>824</v>
+      </c>
+      <c r="C89" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>2008</v>
+      </c>
+      <c r="B90" t="s">
+        <v>825</v>
+      </c>
+      <c r="C90" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>2008</v>
+      </c>
+      <c r="B91" t="s">
+        <v>826</v>
+      </c>
+      <c r="C91" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>2008</v>
+      </c>
+      <c r="B92" t="s">
+        <v>827</v>
+      </c>
+      <c r="C92" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>2008</v>
+      </c>
+      <c r="B93" t="s">
+        <v>828</v>
+      </c>
+      <c r="C93" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>2008</v>
+      </c>
+      <c r="B94" t="s">
+        <v>829</v>
+      </c>
+      <c r="C94" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>2008</v>
+      </c>
+      <c r="B95" t="s">
+        <v>740</v>
+      </c>
+      <c r="C95" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>2008</v>
+      </c>
+      <c r="B96" t="s">
+        <v>741</v>
+      </c>
+      <c r="C96" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>2008</v>
+      </c>
+      <c r="B97" t="s">
+        <v>742</v>
+      </c>
+      <c r="C97" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>2010</v>
+      </c>
+      <c r="B98" t="s">
+        <v>830</v>
+      </c>
+      <c r="C98" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>2010</v>
+      </c>
+      <c r="B99" t="s">
+        <v>831</v>
+      </c>
+      <c r="C99" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>2010</v>
+      </c>
+      <c r="B100" t="s">
+        <v>832</v>
+      </c>
+      <c r="C100" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>2010</v>
+      </c>
+      <c r="B101" t="s">
+        <v>833</v>
+      </c>
+      <c r="C101" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>2010</v>
+      </c>
+      <c r="B102" t="s">
+        <v>834</v>
+      </c>
+      <c r="C102" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>2010</v>
+      </c>
+      <c r="B103" t="s">
+        <v>835</v>
+      </c>
+      <c r="C103" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>2010</v>
+      </c>
+      <c r="B104" t="s">
+        <v>836</v>
+      </c>
+      <c r="C104" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>2010</v>
+      </c>
+      <c r="B105" t="s">
+        <v>837</v>
+      </c>
+      <c r="C105" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>2010</v>
+      </c>
+      <c r="B106" t="s">
+        <v>838</v>
+      </c>
+      <c r="C106" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>2010</v>
+      </c>
+      <c r="B107" t="s">
+        <v>839</v>
+      </c>
+      <c r="C107" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>2010</v>
+      </c>
+      <c r="B108" t="s">
+        <v>840</v>
+      </c>
+      <c r="C108" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>2010</v>
+      </c>
+      <c r="B109" t="s">
+        <v>841</v>
+      </c>
+      <c r="C109" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>2010</v>
+      </c>
+      <c r="B110" t="s">
+        <v>842</v>
+      </c>
+      <c r="C110" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>2010</v>
+      </c>
+      <c r="B111" t="s">
+        <v>843</v>
+      </c>
+      <c r="C111" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>2010</v>
+      </c>
+      <c r="B112" t="s">
+        <v>844</v>
+      </c>
+      <c r="C112" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>2010</v>
+      </c>
+      <c r="B113" t="s">
+        <v>845</v>
+      </c>
+      <c r="C113" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>2010</v>
+      </c>
+      <c r="B114" t="s">
+        <v>846</v>
+      </c>
+      <c r="C114" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>2010</v>
+      </c>
+      <c r="B115" t="s">
+        <v>847</v>
+      </c>
+      <c r="C115" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>2010</v>
+      </c>
+      <c r="B116" t="s">
+        <v>848</v>
+      </c>
+      <c r="C116" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>2010</v>
+      </c>
+      <c r="B117" t="s">
+        <v>849</v>
+      </c>
+      <c r="C117" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>2010</v>
+      </c>
+      <c r="B118" t="s">
+        <v>850</v>
+      </c>
+      <c r="C118" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>2010</v>
+      </c>
+      <c r="B119" t="s">
+        <v>851</v>
+      </c>
+      <c r="C119" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>2010</v>
+      </c>
+      <c r="B120" t="s">
+        <v>852</v>
+      </c>
+      <c r="C120" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>2010</v>
+      </c>
+      <c r="B121" t="s">
+        <v>853</v>
+      </c>
+      <c r="C121" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>2010</v>
+      </c>
+      <c r="B122" t="s">
+        <v>854</v>
+      </c>
+      <c r="C122" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>2010</v>
+      </c>
+      <c r="B123" t="s">
+        <v>855</v>
+      </c>
+      <c r="C123" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>2010</v>
+      </c>
+      <c r="B124" t="s">
+        <v>856</v>
+      </c>
+      <c r="C124" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>2010</v>
+      </c>
+      <c r="B125" t="s">
+        <v>857</v>
+      </c>
+      <c r="C125" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>2010</v>
+      </c>
+      <c r="B126" t="s">
+        <v>858</v>
+      </c>
+      <c r="C126" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>2010</v>
+      </c>
+      <c r="B127" t="s">
+        <v>740</v>
+      </c>
+      <c r="C127" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>2010</v>
+      </c>
+      <c r="B128" t="s">
+        <v>741</v>
+      </c>
+      <c r="C128" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>2010</v>
+      </c>
+      <c r="B129" t="s">
+        <v>742</v>
+      </c>
+      <c r="C129" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>2012</v>
+      </c>
+      <c r="B130" t="s">
+        <v>859</v>
+      </c>
+      <c r="C130" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>2012</v>
+      </c>
+      <c r="B131" t="s">
+        <v>860</v>
+      </c>
+      <c r="C131" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>2012</v>
+      </c>
+      <c r="B132" t="s">
+        <v>861</v>
+      </c>
+      <c r="C132" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>2012</v>
+      </c>
+      <c r="B133" t="s">
+        <v>862</v>
+      </c>
+      <c r="C133" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>2012</v>
+      </c>
+      <c r="B134" t="s">
+        <v>863</v>
+      </c>
+      <c r="C134" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>2012</v>
+      </c>
+      <c r="B135" t="s">
+        <v>864</v>
+      </c>
+      <c r="C135" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>2012</v>
+      </c>
+      <c r="B136" t="s">
+        <v>865</v>
+      </c>
+      <c r="C136" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>2012</v>
+      </c>
+      <c r="B137" t="s">
+        <v>866</v>
+      </c>
+      <c r="C137" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>2012</v>
+      </c>
+      <c r="B138" t="s">
+        <v>867</v>
+      </c>
+      <c r="C138" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>2012</v>
+      </c>
+      <c r="B139" t="s">
+        <v>868</v>
+      </c>
+      <c r="C139" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>2012</v>
+      </c>
+      <c r="B140" t="s">
+        <v>869</v>
+      </c>
+      <c r="C140" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>2012</v>
+      </c>
+      <c r="B141" t="s">
+        <v>870</v>
+      </c>
+      <c r="C141" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>2012</v>
+      </c>
+      <c r="B142" t="s">
+        <v>871</v>
+      </c>
+      <c r="C142" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>2012</v>
+      </c>
+      <c r="B143" t="s">
+        <v>872</v>
+      </c>
+      <c r="C143" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>2012</v>
+      </c>
+      <c r="B144" t="s">
+        <v>873</v>
+      </c>
+      <c r="C144" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>2012</v>
+      </c>
+      <c r="B145" t="s">
+        <v>874</v>
+      </c>
+      <c r="C145" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>2012</v>
+      </c>
+      <c r="B146" t="s">
+        <v>875</v>
+      </c>
+      <c r="C146" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>2012</v>
+      </c>
+      <c r="B147" t="s">
+        <v>876</v>
+      </c>
+      <c r="C147" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>2012</v>
+      </c>
+      <c r="B148" t="s">
+        <v>877</v>
+      </c>
+      <c r="C148" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>2012</v>
+      </c>
+      <c r="B149" t="s">
+        <v>878</v>
+      </c>
+      <c r="C149" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>2012</v>
+      </c>
+      <c r="B150" t="s">
+        <v>879</v>
+      </c>
+      <c r="C150" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>2012</v>
+      </c>
+      <c r="B151" t="s">
+        <v>880</v>
+      </c>
+      <c r="C151" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>2012</v>
+      </c>
+      <c r="B152" t="s">
+        <v>881</v>
+      </c>
+      <c r="C152" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>2012</v>
+      </c>
+      <c r="B153" t="s">
+        <v>882</v>
+      </c>
+      <c r="C153" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>2012</v>
+      </c>
+      <c r="B154" t="s">
+        <v>883</v>
+      </c>
+      <c r="C154" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>2012</v>
+      </c>
+      <c r="B155" t="s">
+        <v>884</v>
+      </c>
+      <c r="C155" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>2012</v>
+      </c>
+      <c r="B156" t="s">
+        <v>885</v>
+      </c>
+      <c r="C156" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>2012</v>
+      </c>
+      <c r="B157" t="s">
+        <v>886</v>
+      </c>
+      <c r="C157" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>2012</v>
+      </c>
+      <c r="B158" t="s">
+        <v>887</v>
+      </c>
+      <c r="C158" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>2012</v>
+      </c>
+      <c r="B159" t="s">
+        <v>740</v>
+      </c>
+      <c r="C159" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>2012</v>
+      </c>
+      <c r="B160" t="s">
+        <v>741</v>
+      </c>
+      <c r="C160" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>2012</v>
+      </c>
+      <c r="B161" t="s">
+        <v>742</v>
+      </c>
+      <c r="C161" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>2014</v>
+      </c>
+      <c r="B162" t="s">
+        <v>888</v>
+      </c>
+      <c r="C162" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>2014</v>
+      </c>
+      <c r="B163" t="s">
+        <v>889</v>
+      </c>
+      <c r="C163" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>2014</v>
+      </c>
+      <c r="B164" t="s">
+        <v>890</v>
+      </c>
+      <c r="C164" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>2014</v>
+      </c>
+      <c r="B165" t="s">
+        <v>891</v>
+      </c>
+      <c r="C165" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>2014</v>
+      </c>
+      <c r="B166" t="s">
+        <v>892</v>
+      </c>
+      <c r="C166" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>2014</v>
+      </c>
+      <c r="B167" t="s">
+        <v>893</v>
+      </c>
+      <c r="C167" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>2014</v>
+      </c>
+      <c r="B168" t="s">
+        <v>894</v>
+      </c>
+      <c r="C168" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>2014</v>
+      </c>
+      <c r="B169" t="s">
+        <v>895</v>
+      </c>
+      <c r="C169" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>2014</v>
+      </c>
+      <c r="B170" t="s">
+        <v>896</v>
+      </c>
+      <c r="C170" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>2014</v>
+      </c>
+      <c r="B171" t="s">
+        <v>897</v>
+      </c>
+      <c r="C171" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>2014</v>
+      </c>
+      <c r="B172" t="s">
+        <v>898</v>
+      </c>
+      <c r="C172" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>2014</v>
+      </c>
+      <c r="B173" t="s">
+        <v>899</v>
+      </c>
+      <c r="C173" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>2014</v>
+      </c>
+      <c r="B174" t="s">
+        <v>900</v>
+      </c>
+      <c r="C174" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>2014</v>
+      </c>
+      <c r="B175" t="s">
+        <v>901</v>
+      </c>
+      <c r="C175" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>2014</v>
+      </c>
+      <c r="B176" t="s">
+        <v>902</v>
+      </c>
+      <c r="C176" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>2014</v>
+      </c>
+      <c r="B177" t="s">
+        <v>903</v>
+      </c>
+      <c r="C177" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>2014</v>
+      </c>
+      <c r="B178" t="s">
+        <v>904</v>
+      </c>
+      <c r="C178" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>2014</v>
+      </c>
+      <c r="B179" t="s">
+        <v>905</v>
+      </c>
+      <c r="C179" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>2014</v>
+      </c>
+      <c r="B180" t="s">
+        <v>906</v>
+      </c>
+      <c r="C180" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>2014</v>
+      </c>
+      <c r="B181" t="s">
+        <v>907</v>
+      </c>
+      <c r="C181" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>2014</v>
+      </c>
+      <c r="B182" t="s">
+        <v>908</v>
+      </c>
+      <c r="C182" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>2014</v>
+      </c>
+      <c r="B183" t="s">
+        <v>909</v>
+      </c>
+      <c r="C183" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>2014</v>
+      </c>
+      <c r="B184" t="s">
+        <v>910</v>
+      </c>
+      <c r="C184" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>2014</v>
+      </c>
+      <c r="B185" t="s">
+        <v>911</v>
+      </c>
+      <c r="C185" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>2014</v>
+      </c>
+      <c r="B186" t="s">
+        <v>912</v>
+      </c>
+      <c r="C186" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>2014</v>
+      </c>
+      <c r="B187" t="s">
+        <v>913</v>
+      </c>
+      <c r="C187" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>2014</v>
+      </c>
+      <c r="B188" t="s">
+        <v>914</v>
+      </c>
+      <c r="C188" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>2014</v>
+      </c>
+      <c r="B189" t="s">
+        <v>915</v>
+      </c>
+      <c r="C189" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>2014</v>
+      </c>
+      <c r="B190" t="s">
+        <v>916</v>
+      </c>
+      <c r="C190" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>2014</v>
+      </c>
+      <c r="B191" t="s">
+        <v>740</v>
+      </c>
+      <c r="C191" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>2014</v>
+      </c>
+      <c r="B192" t="s">
+        <v>741</v>
+      </c>
+      <c r="C192" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>2014</v>
+      </c>
+      <c r="B193" t="s">
+        <v>742</v>
+      </c>
+      <c r="C193" t="s">
+        <v>742</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E165"/>
   <sheetViews>
@@ -7907,7 +11244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
@@ -8346,7 +11683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -8510,7 +11847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
@@ -9002,564 +12339,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>2004</v>
-      </c>
-      <c r="B2" t="s">
-        <v>614</v>
-      </c>
-      <c r="C2" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2004</v>
-      </c>
-      <c r="B3" t="s">
-        <v>615</v>
-      </c>
-      <c r="C3" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2004</v>
-      </c>
-      <c r="B4" t="s">
-        <v>616</v>
-      </c>
-      <c r="C4" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2004</v>
-      </c>
-      <c r="B5" t="s">
-        <v>617</v>
-      </c>
-      <c r="C5" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2004</v>
-      </c>
-      <c r="B6" t="s">
-        <v>618</v>
-      </c>
-      <c r="C6" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2004</v>
-      </c>
-      <c r="B7" t="s">
-        <v>619</v>
-      </c>
-      <c r="C7" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>2004</v>
-      </c>
-      <c r="B8" t="s">
-        <v>620</v>
-      </c>
-      <c r="C8" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>2004</v>
-      </c>
-      <c r="B9" t="s">
-        <v>621</v>
-      </c>
-      <c r="C9" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>2006</v>
-      </c>
-      <c r="B10" t="s">
-        <v>630</v>
-      </c>
-      <c r="C10" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>2006</v>
-      </c>
-      <c r="B11" t="s">
-        <v>631</v>
-      </c>
-      <c r="C11" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2006</v>
-      </c>
-      <c r="B12" t="s">
-        <v>632</v>
-      </c>
-      <c r="C12" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>2006</v>
-      </c>
-      <c r="B13" t="s">
-        <v>633</v>
-      </c>
-      <c r="C13" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>2006</v>
-      </c>
-      <c r="B14" t="s">
-        <v>634</v>
-      </c>
-      <c r="C14" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>2006</v>
-      </c>
-      <c r="B15" t="s">
-        <v>635</v>
-      </c>
-      <c r="C15" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>2006</v>
-      </c>
-      <c r="B16" t="s">
-        <v>636</v>
-      </c>
-      <c r="C16" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>2006</v>
-      </c>
-      <c r="B17" t="s">
-        <v>637</v>
-      </c>
-      <c r="C17" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>2008</v>
-      </c>
-      <c r="B18" t="s">
-        <v>638</v>
-      </c>
-      <c r="C18" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>2008</v>
-      </c>
-      <c r="B19" t="s">
-        <v>639</v>
-      </c>
-      <c r="C19" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>2008</v>
-      </c>
-      <c r="B20" t="s">
-        <v>640</v>
-      </c>
-      <c r="C20" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>2008</v>
-      </c>
-      <c r="B21" t="s">
-        <v>641</v>
-      </c>
-      <c r="C21" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>2008</v>
-      </c>
-      <c r="B22" t="s">
-        <v>642</v>
-      </c>
-      <c r="C22" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>2008</v>
-      </c>
-      <c r="B23" t="s">
-        <v>643</v>
-      </c>
-      <c r="C23" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>2008</v>
-      </c>
-      <c r="B24" t="s">
-        <v>644</v>
-      </c>
-      <c r="C24" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>2008</v>
-      </c>
-      <c r="B25" t="s">
-        <v>645</v>
-      </c>
-      <c r="C25" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>2010</v>
-      </c>
-      <c r="B26" t="s">
-        <v>646</v>
-      </c>
-      <c r="C26" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>2010</v>
-      </c>
-      <c r="B27" t="s">
-        <v>647</v>
-      </c>
-      <c r="C27" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>2010</v>
-      </c>
-      <c r="B28" t="s">
-        <v>648</v>
-      </c>
-      <c r="C28" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>2010</v>
-      </c>
-      <c r="B29" t="s">
-        <v>649</v>
-      </c>
-      <c r="C29" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>2010</v>
-      </c>
-      <c r="B30" t="s">
-        <v>650</v>
-      </c>
-      <c r="C30" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>2010</v>
-      </c>
-      <c r="B31" t="s">
-        <v>651</v>
-      </c>
-      <c r="C31" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>2010</v>
-      </c>
-      <c r="B32" t="s">
-        <v>652</v>
-      </c>
-      <c r="C32" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>2010</v>
-      </c>
-      <c r="B33" t="s">
-        <v>653</v>
-      </c>
-      <c r="C33" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>2012</v>
-      </c>
-      <c r="B34" t="s">
-        <v>654</v>
-      </c>
-      <c r="C34" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>2012</v>
-      </c>
-      <c r="B35" t="s">
-        <v>655</v>
-      </c>
-      <c r="C35" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>2012</v>
-      </c>
-      <c r="B36" t="s">
-        <v>656</v>
-      </c>
-      <c r="C36" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>2012</v>
-      </c>
-      <c r="B37" t="s">
-        <v>657</v>
-      </c>
-      <c r="C37" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>2012</v>
-      </c>
-      <c r="B38" t="s">
-        <v>658</v>
-      </c>
-      <c r="C38" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>2012</v>
-      </c>
-      <c r="B39" t="s">
-        <v>659</v>
-      </c>
-      <c r="C39" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>2012</v>
-      </c>
-      <c r="B40" t="s">
-        <v>660</v>
-      </c>
-      <c r="C40" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>2012</v>
-      </c>
-      <c r="B41" t="s">
-        <v>661</v>
-      </c>
-      <c r="C41" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>2014</v>
-      </c>
-      <c r="B42" t="s">
-        <v>662</v>
-      </c>
-      <c r="C42" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>2014</v>
-      </c>
-      <c r="B43" t="s">
-        <v>663</v>
-      </c>
-      <c r="C43" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>2014</v>
-      </c>
-      <c r="B44" t="s">
-        <v>664</v>
-      </c>
-      <c r="C44" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>2014</v>
-      </c>
-      <c r="B45" t="s">
-        <v>665</v>
-      </c>
-      <c r="C45" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>2014</v>
-      </c>
-      <c r="B46" t="s">
-        <v>666</v>
-      </c>
-      <c r="C46" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>2014</v>
-      </c>
-      <c r="B47" t="s">
-        <v>667</v>
-      </c>
-      <c r="C47" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>2014</v>
-      </c>
-      <c r="B48" t="s">
-        <v>668</v>
-      </c>
-      <c r="C48" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>2014</v>
-      </c>
-      <c r="B49" t="s">
-        <v>669</v>
-      </c>
-      <c r="C49" t="s">
-        <v>629</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
B053 removed for 2014
</commit_message>
<xml_diff>
--- a/data-phi-free/raw/renaming-rules/renaming-rules.xlsx
+++ b/data-phi-free/raw/renaming-rules/renaming-rules.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="911">
   <si>
     <t>year</t>
   </si>
@@ -2765,9 +2765,6 @@
   </si>
   <si>
     <t>ob082</t>
-  </si>
-  <si>
-    <t>ob053</t>
   </si>
   <si>
     <t>ob054</t>
@@ -7245,10 +7242,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E193"/>
+  <dimension ref="A1:E192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="A186" sqref="A186:XFD186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7589,7 +7586,7 @@
         <v>2004</v>
       </c>
       <c r="B30" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C30" t="s">
         <v>739</v>
@@ -7941,7 +7938,7 @@
         <v>2006</v>
       </c>
       <c r="B62" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C62" t="s">
         <v>739</v>
@@ -8293,7 +8290,7 @@
         <v>2008</v>
       </c>
       <c r="B94" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C94" t="s">
         <v>739</v>
@@ -8645,7 +8642,7 @@
         <v>2010</v>
       </c>
       <c r="B126" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C126" t="s">
         <v>739</v>
@@ -8997,7 +8994,7 @@
         <v>2012</v>
       </c>
       <c r="B158" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C158" t="s">
         <v>739</v>
@@ -9308,7 +9305,7 @@
         <v>907</v>
       </c>
       <c r="C186" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
@@ -9319,7 +9316,7 @@
         <v>908</v>
       </c>
       <c r="C187" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
@@ -9330,7 +9327,7 @@
         <v>909</v>
       </c>
       <c r="C188" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
@@ -9341,7 +9338,7 @@
         <v>910</v>
       </c>
       <c r="C189" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
@@ -9349,10 +9346,10 @@
         <v>2014</v>
       </c>
       <c r="B190" t="s">
-        <v>911</v>
+        <v>740</v>
       </c>
       <c r="C190" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
@@ -9360,10 +9357,10 @@
         <v>2014</v>
       </c>
       <c r="B191" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C191" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
@@ -9371,20 +9368,9 @@
         <v>2014</v>
       </c>
       <c r="B192" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C192" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A193">
-        <v>2014</v>
-      </c>
-      <c r="B193" t="s">
-        <v>742</v>
-      </c>
-      <c r="C193" t="s">
         <v>742</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Gender removed from 2014
</commit_message>
<xml_diff>
--- a/data-phi-free/raw/renaming-rules/renaming-rules.xlsx
+++ b/data-phi-free/raw/renaming-rules/renaming-rules.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="911">
   <si>
     <t>year</t>
   </si>
@@ -7242,10 +7242,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E192"/>
+  <dimension ref="A1:E191"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="A186" sqref="A186:XFD186"/>
+      <selection activeCell="A189" sqref="A189:XFD189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9335,10 +9335,10 @@
         <v>2014</v>
       </c>
       <c r="B189" t="s">
-        <v>910</v>
+        <v>740</v>
       </c>
       <c r="C189" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
@@ -9346,10 +9346,10 @@
         <v>2014</v>
       </c>
       <c r="B190" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C190" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
@@ -9357,20 +9357,9 @@
         <v>2014</v>
       </c>
       <c r="B191" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C191" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A192">
-        <v>2014</v>
-      </c>
-      <c r="B192" t="s">
-        <v>742</v>
-      </c>
-      <c r="C192" t="s">
         <v>742</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Social support and social networks scales added
Social support and social network added to scale assembly but not
completed. Error in renaming rules corrected.
</commit_message>
<xml_diff>
--- a/data-phi-free/raw/renaming-rules/renaming-rules.xlsx
+++ b/data-phi-free/raw/renaming-rules/renaming-rules.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21060" activeTab="4"/>
+    <workbookView xWindow="1580" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="loneliness" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="911">
   <si>
     <t>year</t>
   </si>
@@ -2812,9 +2812,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -4636,14 +4635,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -4660,7 +4659,7 @@
       <c r="A2">
         <v>2004</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C2" t="s">
@@ -4671,7 +4670,7 @@
       <c r="A3">
         <v>2004</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C3" t="s">
@@ -4682,7 +4681,7 @@
       <c r="A4">
         <v>2004</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C4" t="s">
@@ -4693,7 +4692,7 @@
       <c r="A5">
         <v>2004</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C5" t="s">
@@ -4704,7 +4703,7 @@
       <c r="A6">
         <v>2004</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C6" t="s">
@@ -4715,7 +4714,7 @@
       <c r="A7">
         <v>2006</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C7" t="s">
@@ -4726,7 +4725,7 @@
       <c r="A8">
         <v>2006</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C8" t="s">
@@ -4737,7 +4736,7 @@
       <c r="A9">
         <v>2006</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C9" t="s">
@@ -4748,7 +4747,7 @@
       <c r="A10">
         <v>2006</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C10" t="s">
@@ -4759,7 +4758,7 @@
       <c r="A11">
         <v>2006</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C11" t="s">
@@ -4770,7 +4769,7 @@
       <c r="A12">
         <v>2008</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C12" t="s">
@@ -4781,7 +4780,7 @@
       <c r="A13">
         <v>2008</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C13" t="s">
@@ -4792,7 +4791,7 @@
       <c r="A14">
         <v>2008</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C14" t="s">
@@ -4803,7 +4802,7 @@
       <c r="A15">
         <v>2008</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C15" t="s">
@@ -4814,7 +4813,7 @@
       <c r="A16">
         <v>2008</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C16" t="s">
@@ -4825,7 +4824,7 @@
       <c r="A17">
         <v>2010</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C17" t="s">
@@ -4836,7 +4835,7 @@
       <c r="A18">
         <v>2010</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C18" t="s">
@@ -4847,7 +4846,7 @@
       <c r="A19">
         <v>2010</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C19" t="s">
@@ -4858,7 +4857,7 @@
       <c r="A20">
         <v>2010</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C20" t="s">
@@ -4869,7 +4868,7 @@
       <c r="A21">
         <v>2010</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C21" t="s">
@@ -4880,7 +4879,7 @@
       <c r="A22">
         <v>2012</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C22" t="s">
@@ -4891,7 +4890,7 @@
       <c r="A23">
         <v>2012</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C23" t="s">
@@ -4902,7 +4901,7 @@
       <c r="A24">
         <v>2012</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C24" t="s">
@@ -4913,7 +4912,7 @@
       <c r="A25">
         <v>2012</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C25" t="s">
@@ -4924,7 +4923,7 @@
       <c r="A26">
         <v>2012</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C26" t="s">
@@ -4935,7 +4934,7 @@
       <c r="A27">
         <v>2014</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C27" t="s">
@@ -4946,7 +4945,7 @@
       <c r="A28">
         <v>2014</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C28" t="s">
@@ -4957,7 +4956,7 @@
       <c r="A29">
         <v>2014</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C29" t="s">
@@ -4968,7 +4967,7 @@
       <c r="A30">
         <v>2014</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C30" t="s">
@@ -4979,7 +4978,7 @@
       <c r="A31">
         <v>2014</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C31" t="s">
@@ -4993,10 +4992,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D110"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5204,1013 +5203,749 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>173</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>174</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>175</v>
       </c>
       <c r="C21" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B22" t="s">
-        <v>132</v>
+        <v>176</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>177</v>
       </c>
       <c r="C23" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B24" t="s">
-        <v>136</v>
+        <v>178</v>
       </c>
       <c r="C24" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
+        <v>179</v>
       </c>
       <c r="C25" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B26" t="s">
-        <v>139</v>
+        <v>180</v>
       </c>
       <c r="C26" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B27" t="s">
-        <v>141</v>
+        <v>181</v>
       </c>
       <c r="C27" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B28" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
       <c r="C28" t="s">
-        <v>144</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>2004</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>145</v>
+        <v>2006</v>
+      </c>
+      <c r="B29" t="s">
+        <v>183</v>
       </c>
       <c r="C29" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>2004</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>147</v>
+        <v>2006</v>
+      </c>
+      <c r="B30" t="s">
+        <v>184</v>
       </c>
       <c r="C30" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>2004</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>149</v>
+        <v>2006</v>
+      </c>
+      <c r="B31" t="s">
+        <v>185</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>2004</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>151</v>
+        <v>2006</v>
+      </c>
+      <c r="B32" t="s">
+        <v>186</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>2004</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>154</v>
+        <v>2006</v>
+      </c>
+      <c r="B33" t="s">
+        <v>187</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B34" t="s">
-        <v>155</v>
+        <v>188</v>
       </c>
       <c r="C34" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B35" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="B36" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="C36" t="s">
-        <v>160</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="B37" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
       <c r="C37" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="B38" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="C38" t="s">
-        <v>164</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="B39" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="C39" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="B40" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="C40" t="s">
-        <v>168</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="B41" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="C41" t="s">
-        <v>170</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="B42" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="C42" t="s">
-        <v>171</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B43" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B44" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B45" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B46" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B47" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B48" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="C48" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B49" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B50" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B51" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="C51" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B52" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B53" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="C53" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B54" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="C54" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B55" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="C55" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B56" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="C56" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B57" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="C57" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B58" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C58" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B59" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C59" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B60" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="C60" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B61" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="C61" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B62" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="C62" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B63" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="C63" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B64" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="C64" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B65" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="C65" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B66" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="C66" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B67" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="C67" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B68" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="C68" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B69" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="C69" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B70" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="C70" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B71" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="C71" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B72" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="C72" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B73" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="C73" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B74" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="C74" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B75" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="C75" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B76" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="C76" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="B77" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="C77" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="B78" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="C78" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="B79" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="C79" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="B80" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="C80" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="B81" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="C81" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="B82" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="C82" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="B83" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="C83" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="B84" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="C84" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="B85" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="C85" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="B86" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="C86" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>2010</v>
-      </c>
-      <c r="B87" t="s">
-        <v>217</v>
-      </c>
-      <c r="C87" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>2010</v>
-      </c>
-      <c r="B88" t="s">
-        <v>218</v>
-      </c>
-      <c r="C88" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>2010</v>
-      </c>
-      <c r="B89" t="s">
-        <v>219</v>
-      </c>
-      <c r="C89" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>2010</v>
-      </c>
-      <c r="B90" t="s">
-        <v>220</v>
-      </c>
-      <c r="C90" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>2010</v>
-      </c>
-      <c r="B91" t="s">
-        <v>221</v>
-      </c>
-      <c r="C91" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>2010</v>
-      </c>
-      <c r="B92" t="s">
-        <v>222</v>
-      </c>
-      <c r="C92" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>2010</v>
-      </c>
-      <c r="B93" t="s">
-        <v>223</v>
-      </c>
-      <c r="C93" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>2012</v>
-      </c>
-      <c r="B94" t="s">
-        <v>224</v>
-      </c>
-      <c r="C94" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>2012</v>
-      </c>
-      <c r="B95" t="s">
-        <v>225</v>
-      </c>
-      <c r="C95" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>2012</v>
-      </c>
-      <c r="B96" t="s">
-        <v>226</v>
-      </c>
-      <c r="C96" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>2012</v>
-      </c>
-      <c r="B97" t="s">
-        <v>227</v>
-      </c>
-      <c r="C97" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>2012</v>
-      </c>
-      <c r="B98" t="s">
-        <v>228</v>
-      </c>
-      <c r="C98" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <v>2012</v>
-      </c>
-      <c r="B99" t="s">
-        <v>229</v>
-      </c>
-      <c r="C99" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <v>2012</v>
-      </c>
-      <c r="B100" t="s">
-        <v>230</v>
-      </c>
-      <c r="C100" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <v>2012</v>
-      </c>
-      <c r="B101" t="s">
-        <v>231</v>
-      </c>
-      <c r="C101" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102">
-        <v>2012</v>
-      </c>
-      <c r="B102" t="s">
-        <v>232</v>
-      </c>
-      <c r="C102" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103">
-        <v>2012</v>
-      </c>
-      <c r="B103" t="s">
-        <v>233</v>
-      </c>
-      <c r="C103" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104">
-        <v>2012</v>
-      </c>
-      <c r="B104" t="s">
-        <v>234</v>
-      </c>
-      <c r="C104" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105">
-        <v>2012</v>
-      </c>
-      <c r="B105" t="s">
-        <v>235</v>
-      </c>
-      <c r="C105" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106">
-        <v>2012</v>
-      </c>
-      <c r="B106" t="s">
-        <v>236</v>
-      </c>
-      <c r="C106" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107">
-        <v>2012</v>
-      </c>
-      <c r="B107" t="s">
-        <v>237</v>
-      </c>
-      <c r="C107" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108">
-        <v>2012</v>
-      </c>
-      <c r="B108" t="s">
-        <v>238</v>
-      </c>
-      <c r="C108" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109">
-        <v>2012</v>
-      </c>
-      <c r="B109" t="s">
-        <v>239</v>
-      </c>
-      <c r="C109" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110">
-        <v>2012</v>
-      </c>
-      <c r="B110" t="s">
-        <v>240</v>
-      </c>
-      <c r="C110" t="s">
         <v>111</v>
       </c>
     </row>
@@ -7244,7 +6979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+    <sheetView topLeftCell="A159" workbookViewId="0">
       <selection activeCell="A189" sqref="A189:XFD189"/>
     </sheetView>
   </sheetViews>
@@ -9372,8 +9107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A138" sqref="A138:A165"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="F159" sqref="F159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9405,6 +9140,9 @@
       <c r="C2" t="s">
         <v>112</v>
       </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -9416,6 +9154,9 @@
       <c r="C3" t="s">
         <v>113</v>
       </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -9427,6 +9168,9 @@
       <c r="C4" t="s">
         <v>114</v>
       </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -9438,6 +9182,9 @@
       <c r="C5" t="s">
         <v>115</v>
       </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -9449,6 +9196,9 @@
       <c r="C6" t="s">
         <v>134</v>
       </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -9460,6 +9210,9 @@
       <c r="C7" t="s">
         <v>135</v>
       </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -9471,6 +9224,9 @@
       <c r="C8" t="s">
         <v>138</v>
       </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -9482,6 +9238,9 @@
       <c r="C9" t="s">
         <v>140</v>
       </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -9493,6 +9252,9 @@
       <c r="C10" t="s">
         <v>142</v>
       </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -9504,6 +9266,9 @@
       <c r="C11" t="s">
         <v>144</v>
       </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -9515,6 +9280,9 @@
       <c r="C12" t="s">
         <v>146</v>
       </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -9526,6 +9294,9 @@
       <c r="C13" t="s">
         <v>148</v>
       </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -9537,6 +9308,9 @@
       <c r="C14" t="s">
         <v>150</v>
       </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -9548,6 +9322,9 @@
       <c r="C15" t="s">
         <v>152</v>
       </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -9559,8 +9336,11 @@
       <c r="C16" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2004</v>
       </c>
@@ -9570,8 +9350,11 @@
       <c r="C17" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2004</v>
       </c>
@@ -9581,8 +9364,11 @@
       <c r="C18" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2004</v>
       </c>
@@ -9592,8 +9378,11 @@
       <c r="C19" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2004</v>
       </c>
@@ -9603,8 +9392,11 @@
       <c r="C20" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2004</v>
       </c>
@@ -9614,8 +9406,11 @@
       <c r="C21" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2004</v>
       </c>
@@ -9625,8 +9420,11 @@
       <c r="C22" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2004</v>
       </c>
@@ -9636,8 +9434,11 @@
       <c r="C23" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2004</v>
       </c>
@@ -9647,8 +9448,11 @@
       <c r="C24" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2004</v>
       </c>
@@ -9658,8 +9462,11 @@
       <c r="C25" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2006</v>
       </c>
@@ -9669,8 +9476,11 @@
       <c r="C26" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2006</v>
       </c>
@@ -9680,8 +9490,11 @@
       <c r="C27" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2006</v>
       </c>
@@ -9691,8 +9504,11 @@
       <c r="C28" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2006</v>
       </c>
@@ -9702,8 +9518,11 @@
       <c r="C29" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2006</v>
       </c>
@@ -9713,8 +9532,11 @@
       <c r="C30" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2006</v>
       </c>
@@ -9724,8 +9546,11 @@
       <c r="C31" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2006</v>
       </c>
@@ -9735,8 +9560,11 @@
       <c r="C32" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2006</v>
       </c>
@@ -9746,8 +9574,11 @@
       <c r="C33" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2006</v>
       </c>
@@ -9757,8 +9588,11 @@
       <c r="C34" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2006</v>
       </c>
@@ -9768,8 +9602,11 @@
       <c r="C35" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2006</v>
       </c>
@@ -9779,8 +9616,11 @@
       <c r="C36" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2006</v>
       </c>
@@ -9790,8 +9630,11 @@
       <c r="C37" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2006</v>
       </c>
@@ -9801,8 +9644,11 @@
       <c r="C38" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2006</v>
       </c>
@@ -9812,8 +9658,11 @@
       <c r="C39" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2006</v>
       </c>
@@ -9823,8 +9672,11 @@
       <c r="C40" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2006</v>
       </c>
@@ -9834,8 +9686,11 @@
       <c r="C41" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2006</v>
       </c>
@@ -9845,8 +9700,11 @@
       <c r="C42" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2006</v>
       </c>
@@ -9856,8 +9714,11 @@
       <c r="C43" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2006</v>
       </c>
@@ -9867,8 +9728,11 @@
       <c r="C44" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2006</v>
       </c>
@@ -9878,8 +9742,11 @@
       <c r="C45" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2006</v>
       </c>
@@ -9889,8 +9756,11 @@
       <c r="C46" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2006</v>
       </c>
@@ -9900,8 +9770,11 @@
       <c r="C47" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2006</v>
       </c>
@@ -9911,8 +9784,11 @@
       <c r="C48" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2006</v>
       </c>
@@ -9922,8 +9798,11 @@
       <c r="C49" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2006</v>
       </c>
@@ -9933,8 +9812,11 @@
       <c r="C50" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2006</v>
       </c>
@@ -9944,8 +9826,11 @@
       <c r="C51" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2006</v>
       </c>
@@ -9955,8 +9840,11 @@
       <c r="C52" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2006</v>
       </c>
@@ -9966,8 +9854,11 @@
       <c r="C53" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2008</v>
       </c>
@@ -9977,8 +9868,11 @@
       <c r="C54" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2008</v>
       </c>
@@ -9988,8 +9882,11 @@
       <c r="C55" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2008</v>
       </c>
@@ -9999,8 +9896,11 @@
       <c r="C56" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2008</v>
       </c>
@@ -10010,8 +9910,11 @@
       <c r="C57" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2008</v>
       </c>
@@ -10021,8 +9924,11 @@
       <c r="C58" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2008</v>
       </c>
@@ -10032,8 +9938,11 @@
       <c r="C59" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2008</v>
       </c>
@@ -10043,8 +9952,11 @@
       <c r="C60" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2008</v>
       </c>
@@ -10054,8 +9966,11 @@
       <c r="C61" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2008</v>
       </c>
@@ -10065,8 +9980,11 @@
       <c r="C62" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2008</v>
       </c>
@@ -10076,8 +9994,11 @@
       <c r="C63" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2008</v>
       </c>
@@ -10087,8 +10008,11 @@
       <c r="C64" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2008</v>
       </c>
@@ -10098,8 +10022,11 @@
       <c r="C65" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2008</v>
       </c>
@@ -10109,8 +10036,11 @@
       <c r="C66" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2008</v>
       </c>
@@ -10120,8 +10050,11 @@
       <c r="C67" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2008</v>
       </c>
@@ -10131,8 +10064,11 @@
       <c r="C68" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2008</v>
       </c>
@@ -10142,8 +10078,11 @@
       <c r="C69" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2008</v>
       </c>
@@ -10153,8 +10092,11 @@
       <c r="C70" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2008</v>
       </c>
@@ -10164,8 +10106,11 @@
       <c r="C71" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2008</v>
       </c>
@@ -10175,8 +10120,11 @@
       <c r="C72" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2008</v>
       </c>
@@ -10186,8 +10134,11 @@
       <c r="C73" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2008</v>
       </c>
@@ -10197,8 +10148,11 @@
       <c r="C74" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2008</v>
       </c>
@@ -10208,8 +10162,11 @@
       <c r="C75" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2008</v>
       </c>
@@ -10219,8 +10176,11 @@
       <c r="C76" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2008</v>
       </c>
@@ -10230,8 +10190,11 @@
       <c r="C77" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2008</v>
       </c>
@@ -10241,8 +10204,11 @@
       <c r="C78" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2008</v>
       </c>
@@ -10252,8 +10218,11 @@
       <c r="C79" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2008</v>
       </c>
@@ -10263,8 +10232,11 @@
       <c r="C80" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2008</v>
       </c>
@@ -10274,8 +10246,11 @@
       <c r="C81" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2010</v>
       </c>
@@ -10285,8 +10260,11 @@
       <c r="C82" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2010</v>
       </c>
@@ -10296,8 +10274,11 @@
       <c r="C83" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2010</v>
       </c>
@@ -10307,8 +10288,11 @@
       <c r="C84" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2010</v>
       </c>
@@ -10318,8 +10302,11 @@
       <c r="C85" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2010</v>
       </c>
@@ -10329,8 +10316,11 @@
       <c r="C86" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>2010</v>
       </c>
@@ -10340,8 +10330,11 @@
       <c r="C87" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2010</v>
       </c>
@@ -10351,8 +10344,11 @@
       <c r="C88" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2010</v>
       </c>
@@ -10362,8 +10358,11 @@
       <c r="C89" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2010</v>
       </c>
@@ -10373,8 +10372,11 @@
       <c r="C90" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>2010</v>
       </c>
@@ -10384,8 +10386,11 @@
       <c r="C91" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2010</v>
       </c>
@@ -10395,8 +10400,11 @@
       <c r="C92" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2010</v>
       </c>
@@ -10406,8 +10414,11 @@
       <c r="C93" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>2010</v>
       </c>
@@ -10417,8 +10428,11 @@
       <c r="C94" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>2010</v>
       </c>
@@ -10428,8 +10442,11 @@
       <c r="C95" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>2010</v>
       </c>
@@ -10439,8 +10456,11 @@
       <c r="C96" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2010</v>
       </c>
@@ -10450,8 +10470,11 @@
       <c r="C97" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2010</v>
       </c>
@@ -10461,8 +10484,11 @@
       <c r="C98" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2010</v>
       </c>
@@ -10472,8 +10498,11 @@
       <c r="C99" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>2010</v>
       </c>
@@ -10483,8 +10512,11 @@
       <c r="C100" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2010</v>
       </c>
@@ -10494,8 +10526,11 @@
       <c r="C101" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>2010</v>
       </c>
@@ -10505,8 +10540,11 @@
       <c r="C102" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>2010</v>
       </c>
@@ -10516,8 +10554,11 @@
       <c r="C103" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D103" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2010</v>
       </c>
@@ -10527,8 +10568,11 @@
       <c r="C104" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D104" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2010</v>
       </c>
@@ -10538,8 +10582,11 @@
       <c r="C105" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D105" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>2010</v>
       </c>
@@ -10549,8 +10596,11 @@
       <c r="C106" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D106" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2010</v>
       </c>
@@ -10560,8 +10610,11 @@
       <c r="C107" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>2010</v>
       </c>
@@ -10571,8 +10624,11 @@
       <c r="C108" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>2010</v>
       </c>
@@ -10582,8 +10638,11 @@
       <c r="C109" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>2012</v>
       </c>
@@ -10593,8 +10652,11 @@
       <c r="C110" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D110" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>2012</v>
       </c>
@@ -10604,8 +10666,11 @@
       <c r="C111" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>2012</v>
       </c>
@@ -10615,8 +10680,11 @@
       <c r="C112" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>2012</v>
       </c>
@@ -10626,8 +10694,11 @@
       <c r="C113" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D113" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>2012</v>
       </c>
@@ -10637,8 +10708,11 @@
       <c r="C114" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D114" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>2012</v>
       </c>
@@ -10648,8 +10722,11 @@
       <c r="C115" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D115" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>2012</v>
       </c>
@@ -10659,8 +10736,11 @@
       <c r="C116" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D116" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>2012</v>
       </c>
@@ -10670,8 +10750,11 @@
       <c r="C117" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>2012</v>
       </c>
@@ -10681,8 +10764,11 @@
       <c r="C118" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>2012</v>
       </c>
@@ -10692,8 +10778,11 @@
       <c r="C119" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D119" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>2012</v>
       </c>
@@ -10703,8 +10792,11 @@
       <c r="C120" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D120" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>2012</v>
       </c>
@@ -10714,8 +10806,11 @@
       <c r="C121" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D121" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>2012</v>
       </c>
@@ -10725,8 +10820,11 @@
       <c r="C122" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D122" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>2012</v>
       </c>
@@ -10736,8 +10834,11 @@
       <c r="C123" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D123" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>2012</v>
       </c>
@@ -10747,8 +10848,11 @@
       <c r="C124" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D124" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>2012</v>
       </c>
@@ -10758,8 +10862,11 @@
       <c r="C125" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D125" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>2012</v>
       </c>
@@ -10769,8 +10876,11 @@
       <c r="C126" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D126" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>2012</v>
       </c>
@@ -10780,8 +10890,11 @@
       <c r="C127" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D127" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>2012</v>
       </c>
@@ -10791,8 +10904,11 @@
       <c r="C128" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D128" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>2012</v>
       </c>
@@ -10802,8 +10918,11 @@
       <c r="C129" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D129" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>2012</v>
       </c>
@@ -10813,8 +10932,11 @@
       <c r="C130" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D130" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>2012</v>
       </c>
@@ -10824,8 +10946,11 @@
       <c r="C131" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>2012</v>
       </c>
@@ -10835,8 +10960,11 @@
       <c r="C132" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D132" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>2012</v>
       </c>
@@ -10846,8 +10974,11 @@
       <c r="C133" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>2012</v>
       </c>
@@ -10857,8 +10988,11 @@
       <c r="C134" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>2012</v>
       </c>
@@ -10868,8 +11002,11 @@
       <c r="C135" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D135" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>2012</v>
       </c>
@@ -10879,8 +11016,11 @@
       <c r="C136" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D136" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>2012</v>
       </c>
@@ -10890,8 +11030,11 @@
       <c r="C137" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D137" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>2014</v>
       </c>
@@ -10901,8 +11044,11 @@
       <c r="C138" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D138" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>2014</v>
       </c>
@@ -10912,8 +11058,11 @@
       <c r="C139" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D139" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>2014</v>
       </c>
@@ -10923,8 +11072,11 @@
       <c r="C140" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D140" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>2014</v>
       </c>
@@ -10934,8 +11086,11 @@
       <c r="C141" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D141" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>2014</v>
       </c>
@@ -10945,8 +11100,11 @@
       <c r="C142" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D142" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>2014</v>
       </c>
@@ -10956,8 +11114,11 @@
       <c r="C143" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D143" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>2014</v>
       </c>
@@ -10967,8 +11128,11 @@
       <c r="C144" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D144" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>2014</v>
       </c>
@@ -10978,8 +11142,11 @@
       <c r="C145" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>2014</v>
       </c>
@@ -10989,8 +11156,11 @@
       <c r="C146" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D146" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>2014</v>
       </c>
@@ -11000,8 +11170,11 @@
       <c r="C147" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D147" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>2014</v>
       </c>
@@ -11011,8 +11184,11 @@
       <c r="C148" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D148" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>2014</v>
       </c>
@@ -11022,8 +11198,11 @@
       <c r="C149" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>2014</v>
       </c>
@@ -11033,8 +11212,11 @@
       <c r="C150" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D150" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>2014</v>
       </c>
@@ -11044,8 +11226,11 @@
       <c r="C151" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D151" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>2014</v>
       </c>
@@ -11055,8 +11240,11 @@
       <c r="C152" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D152" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>2014</v>
       </c>
@@ -11066,8 +11254,11 @@
       <c r="C153" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D153" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>2014</v>
       </c>
@@ -11077,8 +11268,11 @@
       <c r="C154" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D154" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>2014</v>
       </c>
@@ -11088,8 +11282,11 @@
       <c r="C155" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D155" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>2014</v>
       </c>
@@ -11099,8 +11296,11 @@
       <c r="C156" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D156" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>2014</v>
       </c>
@@ -11110,8 +11310,11 @@
       <c r="C157" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D157" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>2014</v>
       </c>
@@ -11121,8 +11324,11 @@
       <c r="C158" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D158" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>2014</v>
       </c>
@@ -11132,8 +11338,11 @@
       <c r="C159" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D159" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>2014</v>
       </c>
@@ -11143,8 +11352,11 @@
       <c r="C160" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D160" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>2014</v>
       </c>
@@ -11154,8 +11366,11 @@
       <c r="C161" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D161" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>2014</v>
       </c>
@@ -11165,8 +11380,11 @@
       <c r="C162" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D162" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>2014</v>
       </c>
@@ -11176,8 +11394,11 @@
       <c r="C163" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D163" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>2014</v>
       </c>
@@ -11187,8 +11408,11 @@
       <c r="C164" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D164" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>2014</v>
       </c>
@@ -11197,6 +11421,9 @@
       </c>
       <c r="C165" t="s">
         <v>171</v>
+      </c>
+      <c r="D165" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Social network scale added
</commit_message>
<xml_diff>
--- a/data-phi-free/raw/renaming-rules/renaming-rules.xlsx
+++ b/data-phi-free/raw/renaming-rules/renaming-rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="5"/>
+    <workbookView xWindow="8880" yWindow="540" windowWidth="33600" windowHeight="20460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="loneliness" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="911">
   <si>
     <t>year</t>
   </si>
@@ -5125,7 +5125,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView zoomScale="110" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5487,10 +5487,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5599,852 +5599,354 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>173</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>175</v>
       </c>
       <c r="C12" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>177</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>178</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>179</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>180</v>
       </c>
       <c r="C17" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>190</v>
       </c>
       <c r="C18" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B19" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B20" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B21" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B22" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B23" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="C23" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B24" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="B25" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B26" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
       <c r="C26" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B27" t="s">
-        <v>181</v>
+        <v>208</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B28" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B29" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="C29" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B30" t="s">
-        <v>184</v>
+        <v>211</v>
       </c>
       <c r="C30" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B31" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="C31" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B32" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="C32" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B33" t="s">
-        <v>187</v>
+        <v>214</v>
       </c>
       <c r="C33" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="B34" t="s">
-        <v>188</v>
+        <v>224</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="B35" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B36" t="s">
-        <v>190</v>
+        <v>226</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B37" t="s">
-        <v>191</v>
+        <v>227</v>
       </c>
       <c r="C37" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B38" t="s">
-        <v>192</v>
+        <v>228</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B39" t="s">
-        <v>193</v>
+        <v>229</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B40" t="s">
-        <v>194</v>
+        <v>230</v>
       </c>
       <c r="C40" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B41" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>2008</v>
-      </c>
-      <c r="B42" t="s">
-        <v>196</v>
-      </c>
-      <c r="C42" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>2008</v>
-      </c>
-      <c r="B43" t="s">
-        <v>197</v>
-      </c>
-      <c r="C43" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>2008</v>
-      </c>
-      <c r="B44" t="s">
-        <v>198</v>
-      </c>
-      <c r="C44" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>2008</v>
-      </c>
-      <c r="B45" t="s">
-        <v>199</v>
-      </c>
-      <c r="C45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>2008</v>
-      </c>
-      <c r="B46" t="s">
-        <v>200</v>
-      </c>
-      <c r="C46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>2008</v>
-      </c>
-      <c r="B47" t="s">
-        <v>201</v>
-      </c>
-      <c r="C47" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>2008</v>
-      </c>
-      <c r="B48" t="s">
-        <v>202</v>
-      </c>
-      <c r="C48" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>2008</v>
-      </c>
-      <c r="B49" t="s">
-        <v>203</v>
-      </c>
-      <c r="C49" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>2008</v>
-      </c>
-      <c r="B50" t="s">
-        <v>204</v>
-      </c>
-      <c r="C50" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>2008</v>
-      </c>
-      <c r="B51" t="s">
-        <v>205</v>
-      </c>
-      <c r="C51" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>2008</v>
-      </c>
-      <c r="B52" t="s">
-        <v>206</v>
-      </c>
-      <c r="C52" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>2010</v>
-      </c>
-      <c r="B53" t="s">
-        <v>207</v>
-      </c>
-      <c r="C53" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>2010</v>
-      </c>
-      <c r="B54" t="s">
-        <v>208</v>
-      </c>
-      <c r="C54" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>2010</v>
-      </c>
-      <c r="B55" t="s">
-        <v>209</v>
-      </c>
-      <c r="C55" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>2010</v>
-      </c>
-      <c r="B56" t="s">
-        <v>210</v>
-      </c>
-      <c r="C56" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>2010</v>
-      </c>
-      <c r="B57" t="s">
-        <v>211</v>
-      </c>
-      <c r="C57" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>2010</v>
-      </c>
-      <c r="B58" t="s">
-        <v>212</v>
-      </c>
-      <c r="C58" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>2010</v>
-      </c>
-      <c r="B59" t="s">
-        <v>213</v>
-      </c>
-      <c r="C59" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>2010</v>
-      </c>
-      <c r="B60" t="s">
-        <v>214</v>
-      </c>
-      <c r="C60" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>2010</v>
-      </c>
-      <c r="B61" t="s">
-        <v>215</v>
-      </c>
-      <c r="C61" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>2010</v>
-      </c>
-      <c r="B62" t="s">
-        <v>216</v>
-      </c>
-      <c r="C62" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>2010</v>
-      </c>
-      <c r="B63" t="s">
-        <v>217</v>
-      </c>
-      <c r="C63" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>2010</v>
-      </c>
-      <c r="B64" t="s">
-        <v>218</v>
-      </c>
-      <c r="C64" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>2010</v>
-      </c>
-      <c r="B65" t="s">
-        <v>219</v>
-      </c>
-      <c r="C65" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>2010</v>
-      </c>
-      <c r="B66" t="s">
-        <v>220</v>
-      </c>
-      <c r="C66" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>2010</v>
-      </c>
-      <c r="B67" t="s">
-        <v>221</v>
-      </c>
-      <c r="C67" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>2010</v>
-      </c>
-      <c r="B68" t="s">
-        <v>222</v>
-      </c>
-      <c r="C68" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>2010</v>
-      </c>
-      <c r="B69" t="s">
-        <v>223</v>
-      </c>
-      <c r="C69" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>2012</v>
-      </c>
-      <c r="B70" t="s">
-        <v>224</v>
-      </c>
-      <c r="C70" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>2012</v>
-      </c>
-      <c r="B71" t="s">
-        <v>225</v>
-      </c>
-      <c r="C71" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>2012</v>
-      </c>
-      <c r="B72" t="s">
-        <v>226</v>
-      </c>
-      <c r="C72" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>2012</v>
-      </c>
-      <c r="B73" t="s">
-        <v>227</v>
-      </c>
-      <c r="C73" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>2012</v>
-      </c>
-      <c r="B74" t="s">
-        <v>228</v>
-      </c>
-      <c r="C74" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>2012</v>
-      </c>
-      <c r="B75" t="s">
-        <v>229</v>
-      </c>
-      <c r="C75" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>2012</v>
-      </c>
-      <c r="B76" t="s">
-        <v>230</v>
-      </c>
-      <c r="C76" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>2012</v>
-      </c>
-      <c r="B77" t="s">
-        <v>231</v>
-      </c>
-      <c r="C77" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>2012</v>
-      </c>
-      <c r="B78" t="s">
-        <v>232</v>
-      </c>
-      <c r="C78" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>2012</v>
-      </c>
-      <c r="B79" t="s">
-        <v>233</v>
-      </c>
-      <c r="C79" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>2012</v>
-      </c>
-      <c r="B80" t="s">
-        <v>234</v>
-      </c>
-      <c r="C80" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>2012</v>
-      </c>
-      <c r="B81" t="s">
-        <v>235</v>
-      </c>
-      <c r="C81" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>2012</v>
-      </c>
-      <c r="B82" t="s">
-        <v>236</v>
-      </c>
-      <c r="C82" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>2012</v>
-      </c>
-      <c r="B83" t="s">
-        <v>237</v>
-      </c>
-      <c r="C83" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>2012</v>
-      </c>
-      <c r="B84" t="s">
-        <v>238</v>
-      </c>
-      <c r="C84" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>2012</v>
-      </c>
-      <c r="B85" t="s">
-        <v>239</v>
-      </c>
-      <c r="C85" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>2012</v>
-      </c>
-      <c r="B86" t="s">
-        <v>240</v>
-      </c>
-      <c r="C86" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -8136,7 +7638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+    <sheetView topLeftCell="A148" workbookViewId="0">
       <selection activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>

</xml_diff>